<commit_message>
Nueva pagina con entrenadores
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/infromes-KBZA/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE8CEC9-D0BC-A946-B765-39370EC05C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2EF38D-3DB7-6342-A2A6-1EB5DD1D6A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
-    <sheet name="source_informes" sheetId="1" r:id="rId1"/>
+    <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
+    <sheet name="Entrenadores" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="168">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -86,18 +87,12 @@
     <t>Posicion</t>
   </si>
   <si>
-    <t>Nombre_Jugador</t>
-  </si>
-  <si>
     <t>Edad</t>
   </si>
   <si>
     <t>Fecha_Nacimiento</t>
   </si>
   <si>
-    <t>Vencimiento_Contrato</t>
-  </si>
-  <si>
     <t>Transfermarket</t>
   </si>
   <si>
@@ -432,6 +427,120 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=X16KCiIP0yo&amp;t=8s</t>
+  </si>
+  <si>
+    <t>Vencimiento Contrato</t>
+  </si>
+  <si>
+    <t>Nombre Jugador</t>
+  </si>
+  <si>
+    <t>Nombre Entrenador</t>
+  </si>
+  <si>
+    <t>Diego Martinez</t>
+  </si>
+  <si>
+    <t>Esquemas Predilectos</t>
+  </si>
+  <si>
+    <t>Argentino</t>
+  </si>
+  <si>
+    <t>4-3-1-2</t>
+  </si>
+  <si>
+    <t>Nombre Foto Entrenador</t>
+  </si>
+  <si>
+    <t>Fase Ofensiva</t>
+  </si>
+  <si>
+    <t>Nombre Video Fase Ofensiva</t>
+  </si>
+  <si>
+    <t>Fase Defensiva</t>
+  </si>
+  <si>
+    <t>Nombre Video Fase Defensiva</t>
+  </si>
+  <si>
+    <t>Transiciones</t>
+  </si>
+  <si>
+    <t>Nombre Video Otras Observaciones</t>
+  </si>
+  <si>
+    <t>Nombre Foto Ultimos Partidos 1</t>
+  </si>
+  <si>
+    <t>Nombre Foto Ultimos Partidos 2</t>
+  </si>
+  <si>
+    <t>Diego_Martinez</t>
+  </si>
+  <si>
+    <t>Descripción Defensiva Diego Martinez</t>
+  </si>
+  <si>
+    <t>Descripción de Transiciones Diego Martinez</t>
+  </si>
+  <si>
+    <t>Descripción de Otras Observaciones</t>
+  </si>
+  <si>
+    <t>Descripcion Ultimos Partidos Diego Martinez</t>
+  </si>
+  <si>
+    <t>Nombre Foto Escudo</t>
+  </si>
+  <si>
+    <t>Nombre Video Transiciones</t>
+  </si>
+  <si>
+    <t>Ultimos Partidos</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MjY3rue8mR0</t>
+  </si>
+  <si>
+    <t>alineacion_Boca</t>
+  </si>
+  <si>
+    <t>Walter Ribonetto</t>
+  </si>
+  <si>
+    <t>Talleres</t>
+  </si>
+  <si>
+    <t>Walter_Ribonetto</t>
+  </si>
+  <si>
+    <t>Descropción Fase Ofensiva Walter Talleres</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_46zrGz6-Dw</t>
+  </si>
+  <si>
+    <t>3-5-2</t>
+  </si>
+  <si>
+    <t>14/07/80</t>
+  </si>
+  <si>
+    <t>13/15/75</t>
+  </si>
+  <si>
+    <t>Fecha de Nacimiento</t>
+  </si>
+  <si>
+    <t>Otras Observaciones</t>
+  </si>
+  <si>
+    <t>Nombre Foto Carrera Entrenador</t>
+  </si>
+  <si>
+    <t>carrera_Diego_Martinez</t>
   </si>
 </sst>
 </file>
@@ -474,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -491,6 +600,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
-      <selection activeCell="BG2" sqref="BG2:BG4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AY3" sqref="AY3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,22 +990,22 @@
   <sheetData>
     <row r="1" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>15</v>
@@ -904,25 +1014,25 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>3</v>
@@ -931,160 +1041,160 @@
         <v>4</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AX1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:69" ht="34" x14ac:dyDescent="0.2">
@@ -1104,13 +1214,13 @@
         <v>2008</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>12</v>
@@ -1119,13 +1229,13 @@
         <v>80</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L2" s="1">
         <v>20</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N2" s="1">
         <v>1000</v>
@@ -1146,10 +1256,10 @@
         <v>100</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="V2" s="1">
         <v>70</v>
@@ -1167,19 +1277,19 @@
         <v>80</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AF2" s="1">
         <v>90</v>
@@ -1191,25 +1301,25 @@
         <v>90</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AP2" s="1">
         <v>90</v>
@@ -1224,7 +1334,7 @@
         <v>20</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AU2" s="1">
         <v>60</v>
@@ -1233,99 +1343,99 @@
         <v>70</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="BH2" s="1">
         <v>2</v>
       </c>
       <c r="BI2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="BJ2" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="BK2" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="BL2" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BM2" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="BN2" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1">
         <v>2009</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="J3" s="1">
         <v>75</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L3" s="1">
         <v>28</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N3" s="3">
         <v>500000</v>
@@ -1334,7 +1444,7 @@
         <v>30</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="1">
         <v>80</v>
@@ -1343,7 +1453,7 @@
         <v>75</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="T3" s="1">
         <v>90</v>
@@ -1352,7 +1462,7 @@
         <v>85</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W3" s="1">
         <v>70</v>
@@ -1376,16 +1486,16 @@
         <v>35</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AF3" s="1">
         <v>80</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AH3" s="1">
         <v>85</v>
@@ -1397,19 +1507,19 @@
         <v>65</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AP3" s="1">
         <v>70</v>
@@ -1424,7 +1534,7 @@
         <v>30</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AU3" s="1">
         <v>80</v>
@@ -1436,87 +1546,87 @@
         <v>90</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AY3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AZ3" s="1" t="s">
+      <c r="BA3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BC3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BG3" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="BA3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="BB3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BC3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BD3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BE3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BF3" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BG3" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="BH3" s="1">
         <v>1</v>
       </c>
       <c r="BI3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="BJ3" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="BK3" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="J4" s="1">
         <v>75</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L4" s="1">
         <v>28</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="N4" s="3">
         <v>143533</v>
@@ -1525,7 +1635,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="1">
         <v>80</v>
@@ -1534,7 +1644,7 @@
         <v>75</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="T4" s="1">
         <v>90</v>
@@ -1543,7 +1653,7 @@
         <v>85</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W4" s="1">
         <v>70</v>
@@ -1567,16 +1677,16 @@
         <v>35</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AF4" s="1">
         <v>80</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AH4" s="1">
         <v>85</v>
@@ -1588,19 +1698,19 @@
         <v>65</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AP4" s="1">
         <v>70</v>
@@ -1615,7 +1725,7 @@
         <v>30</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AU4" s="1">
         <v>80</v>
@@ -1627,55 +1737,55 @@
         <v>90</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AY4" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AZ4" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BA4" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="BC4" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="BD4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="BE4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="BF4" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="BG4" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="BH4" s="1">
         <v>2</v>
       </c>
       <c r="BI4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BJ4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BK4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BJ4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="BK4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BL4" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="BM4" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="BN4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1685,4 +1795,185 @@
     <ignoredError sqref="M3" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M1" t="s">
+        <v>141</v>
+      </c>
+      <c r="N1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O1" t="s">
+        <v>152</v>
+      </c>
+      <c r="P1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R1" t="s">
+        <v>153</v>
+      </c>
+      <c r="S1" t="s">
+        <v>144</v>
+      </c>
+      <c r="T1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" t="s">
+        <v>167</v>
+      </c>
+      <c r="L2" t="s">
+        <v>147</v>
+      </c>
+      <c r="M2" t="s">
+        <v>154</v>
+      </c>
+      <c r="N2" t="s">
+        <v>148</v>
+      </c>
+      <c r="O2" t="s">
+        <v>154</v>
+      </c>
+      <c r="P2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>154</v>
+      </c>
+      <c r="R2" t="s">
+        <v>150</v>
+      </c>
+      <c r="S2" t="s">
+        <v>155</v>
+      </c>
+      <c r="T2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" t="s">
+        <v>159</v>
+      </c>
+      <c r="K3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agregue plantel y se cambio el excel source_informes
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2EF38D-3DB7-6342-A2A6-1EB5DD1D6A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E6EA7E-07DF-FF4A-936A-8138B8442301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="170">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -541,6 +541,12 @@
   </si>
   <si>
     <t>carrera_Diego_Martinez</t>
+  </si>
+  <si>
+    <t>Nombre Foto Plantel Club</t>
+  </si>
+  <si>
+    <t>Plantel_Rosario_Central</t>
   </si>
 </sst>
 </file>
@@ -1799,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1814,7 +1820,7 @@
     <col min="9" max="9" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -1840,43 +1846,46 @@
         <v>151</v>
       </c>
       <c r="I1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J1" t="s">
         <v>166</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>138</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>139</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>140</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>141</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>142</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>152</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>165</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>143</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>153</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>144</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -1902,37 +1911,40 @@
         <v>120</v>
       </c>
       <c r="I2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" t="s">
         <v>167</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>147</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>154</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>148</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>154</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>149</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>154</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>150</v>
-      </c>
-      <c r="S2" t="s">
-        <v>155</v>
       </c>
       <c r="T2" t="s">
         <v>155</v>
       </c>
+      <c r="U2" t="s">
+        <v>155</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -1957,14 +1969,14 @@
       <c r="H3" t="s">
         <v>157</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>159</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1975,5 +1987,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualizacion base de datos en excel y nube de Agus
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\OneDrive\Documentos\scouting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E6EA7E-07DF-FF4A-936A-8138B8442301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17570BE-B40C-476B-98D5-5F1D42CD1617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="227">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -429,12 +427,6 @@
     <t>https://www.youtube.com/watch?v=X16KCiIP0yo&amp;t=8s</t>
   </si>
   <si>
-    <t>Vencimiento Contrato</t>
-  </si>
-  <si>
-    <t>Nombre Jugador</t>
-  </si>
-  <si>
     <t>Nombre Entrenador</t>
   </si>
   <si>
@@ -537,16 +529,197 @@
     <t>Otras Observaciones</t>
   </si>
   <si>
-    <t>Nombre Foto Carrera Entrenador</t>
-  </si>
-  <si>
-    <t>carrera_Diego_Martinez</t>
-  </si>
-  <si>
-    <t>Nombre Foto Plantel Club</t>
-  </si>
-  <si>
-    <t>Plantel_Rosario_Central</t>
+    <t>Pablo Guede</t>
+  </si>
+  <si>
+    <t>Argentinos Juniors</t>
+  </si>
+  <si>
+    <t>No tiene</t>
+  </si>
+  <si>
+    <t>guede</t>
+  </si>
+  <si>
+    <t>argentinosescudo</t>
+  </si>
+  <si>
+    <t>Pablo Guede no es un entrenador que trabaje sobre un único esquema de juego. Ha alternado cinco esquemas en los últimos 8 partidos.
+Es un equipo que trabaja muy bien en la presión provocando que el rival divida la pelota o intentando anticipar en el medio campo, el equipo aprovecha estas situaciones para verticalizar y generar profundidad ya sea con un pase interiores que aprovechan los delanteros con un desmarque de apoyo y jugando con un volante que llegue de frente. Las transiciones también las aprovechan atacando los espacios a espaldas de los laterales con algún delantero que se recueste hacia la banda.
+Argentinos también es un equipo que intenta elaborar desde la salida, acumulando muchos pases, pero muchas veces les cuesta profundizar. Es un equipo que ocupa muy bien los espacios, pero le cuesta generar un cambio de ritmo que le permita profundizar en las posesiones largas. 
+Muchas veces intentan filtrar al ofensivo a espaldas del contención rival para aparecer como tercer hombre 
+Es un equipo que recupera muchos balones divididos y tras recuperar en mitad de cancha intenta atacar rápidamente los espacios a espaldas de la defensa a algún jugador lanzado. En líneas generales generan más daño con asociaciones y juego interior que desbordando por bandas.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/AzKWy20z1h0</t>
+  </si>
+  <si>
+    <t>guedea1</t>
+  </si>
+  <si>
+    <t>guedea2</t>
+  </si>
+  <si>
+    <t>Vencimiento_Contrato</t>
+  </si>
+  <si>
+    <t>Nombre_Jugador</t>
+  </si>
+  <si>
+    <t>Facundo Sava</t>
+  </si>
+  <si>
+    <t>Atletico Tucuman</t>
+  </si>
+  <si>
+    <t>Gustavo Costas</t>
+  </si>
+  <si>
+    <t>Racing Club</t>
+  </si>
+  <si>
+    <t>gustavocostas</t>
+  </si>
+  <si>
+    <t>racingescudo</t>
+  </si>
+  <si>
+    <t>Julio Vaccari</t>
+  </si>
+  <si>
+    <t>Independiente</t>
+  </si>
+  <si>
+    <t>Martin Demichelis</t>
+  </si>
+  <si>
+    <t>Gustavo Quinteros</t>
+  </si>
+  <si>
+    <t>Daniel Oldra</t>
+  </si>
+  <si>
+    <t>Julio Falcioni</t>
+  </si>
+  <si>
+    <t>Boliviano</t>
+  </si>
+  <si>
+    <t>Barracas Central</t>
+  </si>
+  <si>
+    <t>Alejandro Orfila</t>
+  </si>
+  <si>
+    <t>Belgrano</t>
+  </si>
+  <si>
+    <t>Banfield</t>
+  </si>
+  <si>
+    <t>Godoy Cruz</t>
+  </si>
+  <si>
+    <t>Velez Sarsfield</t>
+  </si>
+  <si>
+    <t>River Plate</t>
+  </si>
+  <si>
+    <t>Juan Cruz Real</t>
+  </si>
+  <si>
+    <t>Central Cordoba</t>
+  </si>
+  <si>
+    <t>Lucas Gonzalez Velez</t>
+  </si>
+  <si>
+    <t>Colombiano</t>
+  </si>
+  <si>
+    <t>Eduardo Dominguez</t>
+  </si>
+  <si>
+    <t>Estudiantes LP</t>
+  </si>
+  <si>
+    <t>Marcelo Mendez</t>
+  </si>
+  <si>
+    <t>Gimansia LP</t>
+  </si>
+  <si>
+    <t>Huracan</t>
+  </si>
+  <si>
+    <t>Frank Kudelka</t>
+  </si>
+  <si>
+    <t>Tigre</t>
+  </si>
+  <si>
+    <t>Sarmiento</t>
+  </si>
+  <si>
+    <t>Union</t>
+  </si>
+  <si>
+    <t>Rosario Central</t>
+  </si>
+  <si>
+    <t>Deportivo Riestra</t>
+  </si>
+  <si>
+    <t>Lanus</t>
+  </si>
+  <si>
+    <t>Defensa y Justicia</t>
+  </si>
+  <si>
+    <t>Independiente Rivadavia</t>
+  </si>
+  <si>
+    <t>Instituto</t>
+  </si>
+  <si>
+    <t>Platense</t>
+  </si>
+  <si>
+    <t>Newell's Old Boys</t>
+  </si>
+  <si>
+    <t>San Lorenzo</t>
+  </si>
+  <si>
+    <t>Leandro Romagnoli</t>
+  </si>
+  <si>
+    <t>Sergio Gomez</t>
+  </si>
+  <si>
+    <t>Diego Dabove</t>
+  </si>
+  <si>
+    <t>Ricardo Zielinski</t>
+  </si>
+  <si>
+    <t>Miguel Angel Russo</t>
+  </si>
+  <si>
+    <t>Alejandro Damonte</t>
+  </si>
+  <si>
+    <t>Sebastian Dominguez</t>
+  </si>
+  <si>
+    <t>Cristian Fabbiani</t>
+  </si>
+  <si>
+    <t>Martin Cicotello</t>
+  </si>
+  <si>
+    <t>Kily Gonzalez</t>
   </si>
 </sst>
 </file>
@@ -589,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -607,6 +780,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,79 +1107,79 @@
   <dimension ref="A1:BQ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AY3" sqref="AY3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="11.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.796875" style="1"/>
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="1"/>
-    <col min="11" max="11" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.796875" style="1"/>
+    <col min="11" max="11" width="16.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.296875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="23.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="31" width="17.6640625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="15.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="17.69921875" style="1" customWidth="1"/>
     <col min="32" max="32" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.296875" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="6.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.83203125" style="1"/>
-    <col min="50" max="51" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="56" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.796875" style="1"/>
+    <col min="50" max="51" width="28.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="30.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="33.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="56" width="27.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="23" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="18.296875" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="30.83203125" style="1" customWidth="1"/>
-    <col min="65" max="65" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="27.83203125" style="1" customWidth="1"/>
+    <col min="62" max="62" width="28.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="30.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="30.796875" style="1" customWidth="1"/>
+    <col min="65" max="65" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="27.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="27.796875" style="1" customWidth="1"/>
     <col min="68" max="68" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="70" max="16384" width="10.83203125" style="1"/>
+    <col min="69" max="69" width="18.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="70" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1032,7 +1215,7 @@
         <v>16</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>130</v>
+        <v>173</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>76</v>
@@ -1203,7 +1386,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:69" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:69" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1403,7 +1586,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
@@ -1594,7 +1777,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -1805,24 +1988,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" customWidth="1"/>
+    <col min="6" max="6" width="19.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1831,25 +2015,25 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" t="s">
         <v>137</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="I1" t="s">
-        <v>168</v>
-      </c>
-      <c r="J1" t="s">
-        <v>166</v>
       </c>
       <c r="K1" t="s">
         <v>138</v>
@@ -1861,132 +2045,440 @@
         <v>140</v>
       </c>
       <c r="N1" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P1" t="s">
         <v>141</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" t="s">
         <v>142</v>
       </c>
-      <c r="P1" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>165</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>143</v>
       </c>
-      <c r="S1" t="s">
-        <v>153</v>
-      </c>
-      <c r="T1" t="s">
-        <v>144</v>
-      </c>
-      <c r="U1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
         <v>133</v>
-      </c>
-      <c r="B2" t="s">
-        <v>135</v>
       </c>
       <c r="C2" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>163</v>
+      <c r="D2" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I2" t="s">
-        <v>169</v>
-      </c>
-      <c r="J2" t="s">
-        <v>167</v>
+      <c r="K2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L2" t="s">
+        <v>152</v>
       </c>
       <c r="M2" t="s">
+        <v>146</v>
+      </c>
+      <c r="N2" t="s">
+        <v>152</v>
+      </c>
+      <c r="O2" t="s">
         <v>147</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>148</v>
+      </c>
+      <c r="R2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>154</v>
       </c>
-      <c r="O2" t="s">
-        <v>148</v>
-      </c>
-      <c r="P2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>149</v>
-      </c>
-      <c r="R2" t="s">
-        <v>154</v>
-      </c>
-      <c r="S2" t="s">
-        <v>150</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" t="s">
         <v>155</v>
       </c>
-      <c r="U2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>162</v>
+      <c r="D3" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="E3">
         <v>40</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" t="s">
         <v>158</v>
       </c>
-      <c r="H3" t="s">
-        <v>157</v>
-      </c>
-      <c r="K3" t="s">
-        <v>159</v>
-      </c>
-      <c r="L3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+    </row>
+    <row r="4" spans="1:19" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="8">
+        <v>27345</v>
+      </c>
+      <c r="E4">
+        <v>49</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J4" t="s">
+        <v>170</v>
+      </c>
+      <c r="R4" t="s">
+        <v>171</v>
+      </c>
+      <c r="S4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="8">
+        <v>27095</v>
+      </c>
+      <c r="E5" s="9">
+        <v>50</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="1"/>
     </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="8">
+        <v>23070</v>
+      </c>
+      <c r="E6">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="8">
+        <v>29411</v>
+      </c>
+      <c r="E7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>226</v>
+      </c>
+      <c r="B20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>224</v>
+      </c>
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" t="s">
+        <v>216</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correccion base de datos agus
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\OneDrive\Documentos\scouting\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17570BE-B40C-476B-98D5-5F1D42CD1617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34600DD-9392-4749-B6F2-8749CC064D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="175">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -564,162 +564,6 @@
   </si>
   <si>
     <t>Nombre_Jugador</t>
-  </si>
-  <si>
-    <t>Facundo Sava</t>
-  </si>
-  <si>
-    <t>Atletico Tucuman</t>
-  </si>
-  <si>
-    <t>Gustavo Costas</t>
-  </si>
-  <si>
-    <t>Racing Club</t>
-  </si>
-  <si>
-    <t>gustavocostas</t>
-  </si>
-  <si>
-    <t>racingescudo</t>
-  </si>
-  <si>
-    <t>Julio Vaccari</t>
-  </si>
-  <si>
-    <t>Independiente</t>
-  </si>
-  <si>
-    <t>Martin Demichelis</t>
-  </si>
-  <si>
-    <t>Gustavo Quinteros</t>
-  </si>
-  <si>
-    <t>Daniel Oldra</t>
-  </si>
-  <si>
-    <t>Julio Falcioni</t>
-  </si>
-  <si>
-    <t>Boliviano</t>
-  </si>
-  <si>
-    <t>Barracas Central</t>
-  </si>
-  <si>
-    <t>Alejandro Orfila</t>
-  </si>
-  <si>
-    <t>Belgrano</t>
-  </si>
-  <si>
-    <t>Banfield</t>
-  </si>
-  <si>
-    <t>Godoy Cruz</t>
-  </si>
-  <si>
-    <t>Velez Sarsfield</t>
-  </si>
-  <si>
-    <t>River Plate</t>
-  </si>
-  <si>
-    <t>Juan Cruz Real</t>
-  </si>
-  <si>
-    <t>Central Cordoba</t>
-  </si>
-  <si>
-    <t>Lucas Gonzalez Velez</t>
-  </si>
-  <si>
-    <t>Colombiano</t>
-  </si>
-  <si>
-    <t>Eduardo Dominguez</t>
-  </si>
-  <si>
-    <t>Estudiantes LP</t>
-  </si>
-  <si>
-    <t>Marcelo Mendez</t>
-  </si>
-  <si>
-    <t>Gimansia LP</t>
-  </si>
-  <si>
-    <t>Huracan</t>
-  </si>
-  <si>
-    <t>Frank Kudelka</t>
-  </si>
-  <si>
-    <t>Tigre</t>
-  </si>
-  <si>
-    <t>Sarmiento</t>
-  </si>
-  <si>
-    <t>Union</t>
-  </si>
-  <si>
-    <t>Rosario Central</t>
-  </si>
-  <si>
-    <t>Deportivo Riestra</t>
-  </si>
-  <si>
-    <t>Lanus</t>
-  </si>
-  <si>
-    <t>Defensa y Justicia</t>
-  </si>
-  <si>
-    <t>Independiente Rivadavia</t>
-  </si>
-  <si>
-    <t>Instituto</t>
-  </si>
-  <si>
-    <t>Platense</t>
-  </si>
-  <si>
-    <t>Newell's Old Boys</t>
-  </si>
-  <si>
-    <t>San Lorenzo</t>
-  </si>
-  <si>
-    <t>Leandro Romagnoli</t>
-  </si>
-  <si>
-    <t>Sergio Gomez</t>
-  </si>
-  <si>
-    <t>Diego Dabove</t>
-  </si>
-  <si>
-    <t>Ricardo Zielinski</t>
-  </si>
-  <si>
-    <t>Miguel Angel Russo</t>
-  </si>
-  <si>
-    <t>Alejandro Damonte</t>
-  </si>
-  <si>
-    <t>Sebastian Dominguez</t>
-  </si>
-  <si>
-    <t>Cristian Fabbiani</t>
-  </si>
-  <si>
-    <t>Martin Cicotello</t>
-  </si>
-  <si>
-    <t>Kily Gonzalez</t>
   </si>
 </sst>
 </file>
@@ -762,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -789,7 +633,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,78 +949,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.796875" style="1"/>
+    <col min="2" max="2" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.796875" style="1"/>
-    <col min="11" max="11" width="16.69921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.69921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.296875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="23.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="31" width="17.69921875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="17.6640625" style="1" customWidth="1"/>
     <col min="32" max="32" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="6.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="6.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.796875" style="1"/>
-    <col min="50" max="51" width="28.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="30.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="33.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="56" width="27.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.83203125" style="1"/>
+    <col min="50" max="51" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="56" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="23" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="28.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="30.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="30.796875" style="1" customWidth="1"/>
-    <col min="65" max="65" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="27.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="27.796875" style="1" customWidth="1"/>
+    <col min="62" max="62" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="30.83203125" style="1" customWidth="1"/>
+    <col min="65" max="65" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="27.83203125" style="1" customWidth="1"/>
     <col min="68" max="68" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="18.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="70" max="16384" width="10.796875" style="1"/>
+    <col min="69" max="69" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="70" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>174</v>
       </c>
@@ -1386,7 +1229,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:69" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:69" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1586,7 +1429,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
@@ -1777,7 +1620,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -1988,23 +1831,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.8984375" customWidth="1"/>
-    <col min="6" max="6" width="19.19921875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>130</v>
       </c>
@@ -2063,7 +1906,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -2116,7 +1959,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>154</v>
       </c>
@@ -2148,7 +1991,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -2186,297 +2029,17 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="8">
-        <v>27095</v>
-      </c>
-      <c r="E5" s="9">
-        <v>50</v>
-      </c>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="4"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D6" s="8">
-        <v>23070</v>
-      </c>
-      <c r="E6">
-        <v>61</v>
-      </c>
-      <c r="G6" t="s">
-        <v>179</v>
-      </c>
-      <c r="H6" t="s">
-        <v>180</v>
-      </c>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D7" s="8">
-        <v>29411</v>
-      </c>
-      <c r="E7">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>183</v>
-      </c>
-      <c r="B8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" t="s">
-        <v>194</v>
-      </c>
-      <c r="E8">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>184</v>
-      </c>
-      <c r="B9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>185</v>
-      </c>
-      <c r="B10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>186</v>
-      </c>
-      <c r="B11" t="s">
-        <v>133</v>
-      </c>
-      <c r="C11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>189</v>
-      </c>
-      <c r="B12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>195</v>
-      </c>
-      <c r="B13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>197</v>
-      </c>
-      <c r="B14" t="s">
-        <v>198</v>
-      </c>
-      <c r="C14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>199</v>
-      </c>
-      <c r="B15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>201</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>204</v>
-      </c>
-      <c r="B17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C17" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>223</v>
-      </c>
-      <c r="B18" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>222</v>
-      </c>
-      <c r="B19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>226</v>
-      </c>
-      <c r="B20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>221</v>
-      </c>
-      <c r="B21" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>224</v>
-      </c>
-      <c r="B22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>220</v>
-      </c>
-      <c r="B23" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>225</v>
-      </c>
-      <c r="B25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>219</v>
-      </c>
-      <c r="B26" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>218</v>
-      </c>
-      <c r="B27" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>217</v>
-      </c>
-      <c r="B29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" t="s">
-        <v>216</v>
-      </c>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correccion base de datos agus parte 2
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34600DD-9392-4749-B6F2-8749CC064D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D7570B-9A0B-B448-8C67-F6B389C9DA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="176">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -564,6 +564,9 @@
   </si>
   <si>
     <t>Nombre_Jugador</t>
+  </si>
+  <si>
+    <t>Nombre Foto Plantel Club</t>
   </si>
 </sst>
 </file>
@@ -949,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1831,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1844,10 +1847,11 @@
     <col min="6" max="6" width="19.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>130</v>
       </c>
@@ -1872,41 +1876,44 @@
       <c r="H1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" t="s">
         <v>136</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>137</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>138</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>139</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>140</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>150</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>163</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>141</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>151</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>142</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -1931,35 +1938,36 @@
       <c r="H2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K2" t="s">
+      <c r="I2" s="1"/>
+      <c r="L2" t="s">
         <v>145</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>152</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>146</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>152</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>147</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>152</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>148</v>
-      </c>
-      <c r="R2" t="s">
-        <v>153</v>
       </c>
       <c r="S2" t="s">
         <v>153</v>
       </c>
+      <c r="T2" t="s">
+        <v>153</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>154</v>
       </c>
@@ -1984,14 +1992,14 @@
       <c r="H3" t="s">
         <v>155</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>157</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -2016,29 +2024,29 @@
       <c r="H4" t="s">
         <v>168</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>170</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>171</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="4"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D7" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correccion base de datos agus parte 3
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D7570B-9A0B-B448-8C67-F6B389C9DA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6557EC5-2D84-D040-A637-335C6946908A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="177">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -427,6 +429,12 @@
     <t>https://www.youtube.com/watch?v=X16KCiIP0yo&amp;t=8s</t>
   </si>
   <si>
+    <t>Vencimiento Contrato</t>
+  </si>
+  <si>
+    <t>Nombre Jugador</t>
+  </si>
+  <si>
     <t>Nombre Entrenador</t>
   </si>
   <si>
@@ -508,9 +516,6 @@
     <t>Walter_Ribonetto</t>
   </si>
   <si>
-    <t>Descropción Fase Ofensiva Walter Talleres</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=_46zrGz6-Dw</t>
   </si>
   <si>
@@ -527,6 +532,12 @@
   </si>
   <si>
     <t>Otras Observaciones</t>
+  </si>
+  <si>
+    <t>Nombre Foto Carrera Entrenador</t>
+  </si>
+  <si>
+    <t>Nombre Foto Plantel Club</t>
   </si>
   <si>
     <t>Pablo Guede</t>
@@ -560,13 +571,7 @@
     <t>guedea2</t>
   </si>
   <si>
-    <t>Vencimiento_Contrato</t>
-  </si>
-  <si>
-    <t>Nombre_Jugador</t>
-  </si>
-  <si>
-    <t>Nombre Foto Plantel Club</t>
+    <t>Descripción Fase Ofensiva Walter Talleres</t>
   </si>
 </sst>
 </file>
@@ -609,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -627,14 +632,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -952,11 +954,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ4"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AY3" sqref="AY3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -1025,7 +1027,7 @@
   <sheetData>
     <row r="1" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1061,7 +1063,7 @@
         <v>16</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>76</v>
@@ -1834,26 +1836,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="6" max="6" width="19.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1862,194 +1862,195 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O1" t="s">
+        <v>142</v>
+      </c>
+      <c r="P1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>164</v>
+      </c>
+      <c r="R1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T1" t="s">
+        <v>144</v>
+      </c>
+      <c r="U1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
         <v>135</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K1" t="s">
-        <v>137</v>
-      </c>
-      <c r="L1" t="s">
-        <v>138</v>
-      </c>
-      <c r="M1" t="s">
-        <v>139</v>
-      </c>
-      <c r="N1" t="s">
-        <v>140</v>
-      </c>
-      <c r="O1" t="s">
-        <v>150</v>
-      </c>
-      <c r="P1" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>141</v>
-      </c>
-      <c r="R1" t="s">
-        <v>151</v>
-      </c>
-      <c r="S1" t="s">
-        <v>142</v>
-      </c>
-      <c r="T1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" t="s">
-        <v>133</v>
       </c>
       <c r="C2" t="s">
         <v>69</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>120</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="L2" t="s">
-        <v>145</v>
-      </c>
       <c r="M2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="N2" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="O2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="P2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="Q2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="R2" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="S2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="T2" t="s">
-        <v>153</v>
+        <v>155</v>
+      </c>
+      <c r="U2" t="s">
+        <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E3">
         <v>40</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" t="s">
         <v>159</v>
       </c>
-      <c r="G3" t="s">
-        <v>156</v>
-      </c>
-      <c r="H3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J3" t="s">
-        <v>157</v>
-      </c>
-      <c r="K3" t="s">
-        <v>158</v>
-      </c>
     </row>
-    <row r="4" spans="1:20" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D4" s="8">
+        <v>168</v>
+      </c>
+      <c r="D4" s="7">
         <v>27345</v>
       </c>
       <c r="E4">
         <v>49</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H4" t="s">
-        <v>168</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K4" t="s">
-        <v>170</v>
-      </c>
-      <c r="S4" t="s">
         <v>171</v>
       </c>
+      <c r="K4" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L4" t="s">
+        <v>173</v>
+      </c>
       <c r="T4" t="s">
-        <v>172</v>
+        <v>174</v>
+      </c>
+      <c r="U4" t="s">
+        <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="4"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D7" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correccion base de datos agus parte 5
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB1FD63-4422-C44C-AE6D-D71AFFF38977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA80B48D-D89F-D544-9C75-CF0B3A00DCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Aceleraciones</t>
+  </si>
+  <si>
+    <t>Derecha</t>
   </si>
   <si>
     <t>Seleccion</t>
@@ -458,6 +461,18 @@
   </si>
   <si>
     <t>Descripción Fase Ofensiva Walter Talleres</t>
+  </si>
+  <si>
+    <t>Johan Rojas GEMELO</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>Nacho Pastore</t>
+  </si>
+  <si>
+    <t>1/5/23</t>
   </si>
 </sst>
 </file>
@@ -835,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
-  <dimension ref="A1:BQ2"/>
+  <dimension ref="A1:BQ3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -910,49 +925,49 @@
   <sheetData>
     <row r="1" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>3</v>
@@ -961,201 +976,201 @@
         <v>4</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="Z1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="AM1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AY1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BN1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AZ1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="BE1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="BP1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="J2" s="1">
         <v>75</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L2" s="1">
         <v>28</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N2" s="2">
         <v>143533</v>
@@ -1164,7 +1179,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="1">
         <v>80</v>
@@ -1173,7 +1188,7 @@
         <v>75</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T2" s="1">
         <v>90</v>
@@ -1182,7 +1197,7 @@
         <v>85</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W2" s="1">
         <v>70</v>
@@ -1206,16 +1221,16 @@
         <v>35</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AF2" s="1">
         <v>80</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AH2" s="1">
         <v>85</v>
@@ -1227,19 +1242,19 @@
         <v>65</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AP2" s="1">
         <v>70</v>
@@ -1254,7 +1269,7 @@
         <v>30</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AU2" s="1">
         <v>80</v>
@@ -1266,55 +1281,255 @@
         <v>90</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="BH2" s="1">
         <v>2</v>
       </c>
       <c r="BI2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BJ2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BL2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1">
+        <v>75</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="1">
+        <v>35</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="N3" s="2">
+        <v>10000</v>
+      </c>
+      <c r="O3" s="1">
+        <v>30</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>80</v>
+      </c>
+      <c r="R3" s="1">
+        <v>75</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" s="1">
+        <v>90</v>
+      </c>
+      <c r="U3" s="1">
+        <v>85</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W3" s="1">
+        <v>70</v>
+      </c>
+      <c r="X3" s="1">
+        <v>75</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>50</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>55</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>95</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>35</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>80</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>85</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>60</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>65</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>70</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>95</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>80</v>
+      </c>
+      <c r="AS3" s="1">
+        <v>30</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AU3" s="1">
+        <v>80</v>
+      </c>
+      <c r="AV3" s="1">
+        <v>70</v>
+      </c>
+      <c r="AW3" s="1">
+        <v>90</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BK2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BL2" s="1" t="s">
+      <c r="BA3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BG3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BH3" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="BM2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="BN2" s="1" t="s">
+      <c r="BJ3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK3" s="1" t="s">
         <v>52</v>
+      </c>
+      <c r="BL3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BM3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN3" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1327,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1342,158 +1557,158 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" t="s">
         <v>128</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q1" t="s">
         <v>127</v>
       </c>
-      <c r="K1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" t="s">
-        <v>102</v>
-      </c>
-      <c r="M1" t="s">
-        <v>103</v>
-      </c>
-      <c r="N1" t="s">
-        <v>104</v>
-      </c>
-      <c r="O1" t="s">
-        <v>105</v>
-      </c>
-      <c r="P1" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>126</v>
-      </c>
       <c r="R1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="T1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I2" s="1"/>
       <c r="M2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="O2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="P2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Q2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="R2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="S2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E3">
         <v>40</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" t="s">
+        <v>139</v>
+      </c>
+      <c r="L3" t="s">
         <v>122</v>
-      </c>
-      <c r="G3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H3" t="s">
-        <v>119</v>
-      </c>
-      <c r="K3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D4" s="6">
         <v>27345</v>
@@ -1502,25 +1717,25 @@
         <v>49</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="T4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="U4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
correccion base de datos agus parte 6, andando
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA80B48D-D89F-D544-9C75-CF0B3A00DCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4643F2-D3BC-8748-936E-CA1E092E9F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="145">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>1/5/23</t>
+  </si>
+  <si>
+    <t>argentinosplantel</t>
   </si>
 </sst>
 </file>
@@ -852,7 +855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1542,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1724,6 +1727,9 @@
       </c>
       <c r="H4" t="s">
         <v>134</v>
+      </c>
+      <c r="I4" t="s">
+        <v>144</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
cambio de tamanio video ofensiva en entrenadores y chequeo vista final entrenadores
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4643F2-D3BC-8748-936E-CA1E092E9F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CD2050-8C02-1F49-BBE8-C67BAC609D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="146">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -476,6 +476,9 @@
   </si>
   <si>
     <t>argentinosplantel</t>
+  </si>
+  <si>
+    <t>guedecarrera</t>
   </si>
 </sst>
 </file>
@@ -1545,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1730,6 +1733,9 @@
       </c>
       <c r="I4" t="s">
         <v>144</v>
+      </c>
+      <c r="J4" t="s">
+        <v>145</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
saco recorte redondo, muevo make_radar a helpers y cambio fecha formato en entrenadores
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CD2050-8C02-1F49-BBE8-C67BAC609D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1C28CF-77DD-9C4B-AC86-F7A8BE19E27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -409,12 +409,6 @@
   </si>
   <si>
     <t>3-5-2</t>
-  </si>
-  <si>
-    <t>14/07/80</t>
-  </si>
-  <si>
-    <t>13/15/75</t>
   </si>
   <si>
     <t>Fecha de Nacimiento</t>
@@ -479,6 +473,15 @@
   </si>
   <si>
     <t>guedecarrera</t>
+  </si>
+  <si>
+    <t>12/11/1974</t>
+  </si>
+  <si>
+    <t>16/11/1978</t>
+  </si>
+  <si>
+    <t>06/07/1974</t>
   </si>
 </sst>
 </file>
@@ -536,11 +539,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1340,7 +1343,7 @@
     </row>
     <row r="3" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>48</v>
@@ -1361,7 +1364,7 @@
         <v>45</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>8</v>
@@ -1376,7 +1379,7 @@
         <v>35</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="N3" s="2">
         <v>10000</v>
@@ -1385,7 +1388,7 @@
         <v>30</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q3" s="1">
         <v>80</v>
@@ -1548,17 +1551,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="5"/>
     <col min="6" max="6" width="19.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="19" max="19" width="38.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -1571,8 +1576,8 @@
       <c r="C1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" t="s">
-        <v>126</v>
+      <c r="D1" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -1587,10 +1592,10 @@
         <v>115</v>
       </c>
       <c r="I1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K1" t="s">
         <v>102</v>
@@ -1611,7 +1616,7 @@
         <v>116</v>
       </c>
       <c r="Q1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="R1" t="s">
         <v>107</v>
@@ -1637,10 +1642,10 @@
         <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>100</v>
@@ -1648,7 +1653,7 @@
       <c r="G2" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="7" t="s">
         <v>89</v>
       </c>
       <c r="I2" s="1"/>
@@ -1685,10 +1690,10 @@
         <v>120</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>123</v>
@@ -1700,7 +1705,7 @@
         <v>120</v>
       </c>
       <c r="K3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L3" t="s">
         <v>122</v>
@@ -1708,53 +1713,53 @@
     </row>
     <row r="4" spans="1:21" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
         <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" s="6">
-        <v>27345</v>
+        <v>129</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="E4">
         <v>49</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" t="s">
         <v>132</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>134</v>
       </c>
-      <c r="I4" t="s">
-        <v>144</v>
-      </c>
-      <c r="J4" t="s">
-        <v>145</v>
-      </c>
-      <c r="K4" s="7" t="s">
+      <c r="T4" t="s">
         <v>135</v>
       </c>
-      <c r="L4" t="s">
+      <c r="U4" t="s">
         <v>136</v>
-      </c>
-      <c r="T4" t="s">
-        <v>137</v>
-      </c>
-      <c r="U4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="1"/>
       <c r="F5" s="3"/>
       <c r="G5" s="1"/>

</xml_diff>

<commit_message>
agrego carrera como jugador, agrego circulo y tamaño a foto jugador
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1C28CF-77DD-9C4B-AC86-F7A8BE19E27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2A76E3-6432-8A45-8902-502F9E2C107F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="149">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -482,6 +482,12 @@
   </si>
   <si>
     <t>06/07/1974</t>
+  </si>
+  <si>
+    <t>Nombre Foto Carrera Como Jugador</t>
+  </si>
+  <si>
+    <t>guedecarrerajugador</t>
   </si>
 </sst>
 </file>
@@ -861,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1549,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1563,10 +1569,11 @@
     <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5" customWidth="1"/>
-    <col min="19" max="19" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="29.1640625" customWidth="1"/>
+    <col min="20" max="20" width="38.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -1598,40 +1605,43 @@
         <v>126</v>
       </c>
       <c r="K1" t="s">
+        <v>147</v>
+      </c>
+      <c r="L1" t="s">
         <v>102</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>103</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>104</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>105</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>106</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>125</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>107</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>117</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>108</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1657,29 +1667,29 @@
         <v>89</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>111</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>118</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>112</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>118</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>113</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>118</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -1704,14 +1714,14 @@
       <c r="H3" t="s">
         <v>120</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>137</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -1742,20 +1752,23 @@
       <c r="J4" t="s">
         <v>143</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" t="s">
+        <v>148</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>134</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>135</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
arreglo foto carrera como jugador v1
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FDA9B1-C2A6-134A-81D2-378AD0C51C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D280D6DC-C1B2-804E-8638-A35DE996D9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
@@ -1558,7 +1558,7 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
arreglo bug de path escudo en 00. Cambio de tamanio de escudo para ver si el de San Lorenzo aparece completo
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\OneDrive\Documentos\scouting\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB74E4B-C2ED-49A1-A053-AAD635449910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AD21F6-AA26-1847-8501-57D08E3DA2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="301">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -956,6 +956,9 @@
   </si>
   <si>
     <t>barracascentralescudo</t>
+  </si>
+  <si>
+    <t>Johan Rojas2</t>
   </si>
 </sst>
 </file>
@@ -1345,78 +1348,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ3"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AW2" sqref="AW2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.796875" style="1"/>
+    <col min="2" max="2" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.796875" style="1"/>
-    <col min="11" max="11" width="16.69921875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.69921875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.296875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="23.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="31" width="17.69921875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="17.6640625" style="1" customWidth="1"/>
     <col min="32" max="32" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="6.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="6.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.796875" style="1"/>
-    <col min="50" max="51" width="28.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="30.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="33.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="56" width="27.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.83203125" style="1"/>
+    <col min="50" max="51" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="56" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="23" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="28.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="30.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="30.796875" style="1" customWidth="1"/>
-    <col min="65" max="65" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="27.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="27.796875" style="1" customWidth="1"/>
+    <col min="62" max="62" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="30.83203125" style="1" customWidth="1"/>
+    <col min="65" max="65" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="27.83203125" style="1" customWidth="1"/>
     <col min="68" max="68" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="18.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="70" max="16384" width="10.796875" style="1"/>
+    <col min="69" max="69" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="70" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
@@ -1625,7 +1628,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -1825,10 +1828,205 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.3">
-      <c r="M3" s="4"/>
-      <c r="N3" s="2"/>
-      <c r="BG3" s="1"/>
+    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="1">
+        <v>75</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="1">
+        <v>28</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="2">
+        <v>143533</v>
+      </c>
+      <c r="O3" s="1">
+        <v>30</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>80</v>
+      </c>
+      <c r="R3" s="1">
+        <v>75</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="1">
+        <v>90</v>
+      </c>
+      <c r="U3" s="1">
+        <v>85</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="1">
+        <v>70</v>
+      </c>
+      <c r="X3" s="1">
+        <v>75</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>50</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>55</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>95</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>35</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>60</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>70</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>95</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>80</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU3" s="1">
+        <v>80</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AW3" s="1">
+        <v>90</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BG3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BH3" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BL3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BM3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN3" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1841,23 +2039,24 @@
   <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.19921875" customWidth="1"/>
-    <col min="4" max="4" width="13.296875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.19921875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5" customWidth="1"/>
-    <col min="10" max="11" width="29.19921875" customWidth="1"/>
+    <col min="10" max="11" width="29.1640625" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="6" customWidth="1"/>
     <col min="20" max="20" width="38.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -1891,7 +2090,7 @@
       <c r="K1" t="s">
         <v>135</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="6" t="s">
         <v>100</v>
       </c>
       <c r="M1" t="s">
@@ -1925,7 +2124,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -1963,7 +2162,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -1998,7 +2197,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -2045,7 +2244,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -2077,7 +2276,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -2115,7 +2314,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>144</v>
       </c>
@@ -2147,7 +2346,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="22.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>147</v>
       </c>
@@ -2182,7 +2381,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -2223,7 +2422,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>151</v>
       </c>
@@ -2261,7 +2460,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>153</v>
       </c>
@@ -2290,7 +2489,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>155</v>
       </c>
@@ -2322,7 +2521,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -2354,7 +2553,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>159</v>
       </c>
@@ -2386,7 +2585,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -2433,7 +2632,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2462,7 +2661,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -2491,7 +2690,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>169</v>
       </c>
@@ -2523,7 +2722,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>213</v>
       </c>
@@ -2552,7 +2751,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -2584,7 +2783,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -2616,7 +2815,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>176</v>
       </c>
@@ -2642,7 +2841,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>178</v>
       </c>
@@ -2677,7 +2876,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>180</v>
       </c>
@@ -2703,7 +2902,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -2729,7 +2928,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>184</v>
       </c>
@@ -2758,7 +2957,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>186</v>
       </c>
@@ -2790,19 +2989,19 @@
         <v>274</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D32"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregar jugadores en excel y modificacion de nombres de escudos
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AD21F6-AA26-1847-8501-57D08E3DA2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BD8E7A-B0FE-7046-8EFE-58AF412059D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="307">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -160,9 +160,6 @@
     <t>Velocidad</t>
   </si>
   <si>
-    <t>Agustin Salem</t>
-  </si>
-  <si>
     <t>Pase_Interior_Circulacion</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>Volante Ofensivo</t>
   </si>
   <si>
-    <t>2.3</t>
-  </si>
-  <si>
     <t>Izquierda</t>
   </si>
   <si>
@@ -190,12 +184,6 @@
     <t>Nombre_Video_2</t>
   </si>
   <si>
-    <t>Descripcion Johan Rojas Video 1</t>
-  </si>
-  <si>
-    <t>Descripcion Johan Rojas Video 2</t>
-  </si>
-  <si>
     <t>Cantidad_Videos</t>
   </si>
   <si>
@@ -265,21 +253,6 @@
     <t>Otras_Observaciones</t>
   </si>
   <si>
-    <t xml:space="preserve">Aspectos técnicos de Rojas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aspectos tácticos de Rojas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aspectos físicos de Rojas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personalidad técnicos de Rojas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otras observaciones de Rojas </t>
-  </si>
-  <si>
     <t>Nombre_Video_Compacto</t>
   </si>
   <si>
@@ -293,12 +266,6 @@
   </si>
   <si>
     <t>Aspectos_Fisicos</t>
-  </si>
-  <si>
-    <t>Velez vs Chacarita</t>
-  </si>
-  <si>
-    <t>Velez vs Newels</t>
   </si>
   <si>
     <t>CD_La_Equidad</t>
@@ -716,13 +683,7 @@
     <t>platenseescudo</t>
   </si>
   <si>
-    <t>riverplatescudo</t>
-  </si>
-  <si>
     <t>estudiantesescudo</t>
-  </si>
-  <si>
-    <t>gimansiaescudo</t>
   </si>
   <si>
     <t>rosariocentralescudo</t>
@@ -958,7 +919,66 @@
     <t>barracascentralescudo</t>
   </si>
   <si>
-    <t>Johan Rojas2</t>
+    <t>riverplateescudo</t>
+  </si>
+  <si>
+    <t>gimnasiaescudo</t>
+  </si>
+  <si>
+    <t>Octavio Rivero</t>
+  </si>
+  <si>
+    <t>Lorenzo Albarracin</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Reserva</t>
+  </si>
+  <si>
+    <t>Extremo</t>
+  </si>
+  <si>
+    <t>17/02/2007</t>
+  </si>
+  <si>
+    <t>lorenzoalbarracin</t>
+  </si>
+  <si>
+    <t>https://youtu.be/x0v6x-e6lu4</t>
+  </si>
+  <si>
+    <t>Agustin Lagos</t>
+  </si>
+  <si>
+    <t>Lateral Derecho</t>
+  </si>
+  <si>
+    <t>Derecho</t>
+  </si>
+  <si>
+    <t>09/10/2001</t>
+  </si>
+  <si>
+    <t>31/12/2025</t>
+  </si>
+  <si>
+    <t>Gonzalo Lagos</t>
+  </si>
+  <si>
+    <t>agustinlagos</t>
+  </si>
+  <si>
+    <t>Intervino en todas las fases de juego, tanto en defensa como en la gestación y en la creación del ataque. Es un lateral con gran claridad en el último tercio, con capacidad de pases interiores. Gran técnica en asociaciones en espacios reducidos y en 1 vs 1. Envia centros de primera y en velocidad lo cual es un recurso que sobresale sobre los demás laterales. Es de talla alta y buen porte, gana duelos aeres y es agerrido en la marca. Entiendo los momentos para saltar a la marca. Le faltaría corregir los momentos cuando pasar al ataque ya que deja muchas veces la marca a las espaldas sin tener un espacio claro donde atacar.
+Recibió entre lineas y condujo. Distribuyó y limpio las jugadas. 
+Y sobre todo piso mucho el area!</t>
+  </si>
+  <si>
+    <t>https://youtu.be/XikKxaoU1iw</t>
+  </si>
+  <si>
+    <t>Controles y perfiles para darle continuidad a la jugada. Vision y precision para colocar pases en ventaja. Engaños corporales y habilidad para recibir y girar rápidamente, conducciones en velocidad. Tranquilidad bajo presión, sale gambeta corta.</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1032,6 +1052,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1346,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
-  <dimension ref="A1:BQ3"/>
+  <dimension ref="A1:BQ4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1421,22 +1444,22 @@
   <sheetData>
     <row r="1" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
@@ -1445,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -1457,10 +1480,10 @@
         <v>10</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>12</v>
@@ -1481,7 +1504,7 @@
         <v>31</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>5</v>
@@ -1526,7 +1549,7 @@
         <v>32</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>33</v>
@@ -1568,75 +1591,75 @@
         <v>40</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AY1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AZ1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="BQ1" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>26</v>
@@ -1645,37 +1668,37 @@
         <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="J2" s="1">
         <v>75</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L2" s="1">
         <v>28</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="N2" s="2">
-        <v>143533</v>
+        <v>60</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="O2" s="1">
         <v>4</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>41</v>
+        <v>289</v>
       </c>
       <c r="Q2" s="1">
         <v>80</v>
@@ -1777,105 +1800,69 @@
         <v>90</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BC2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BD2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BE2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BG2" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="BH2" s="1">
-        <v>2</v>
-      </c>
-      <c r="BI2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BJ2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BL2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BM2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN2" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:69" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>291</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>172</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
+      <c r="E3" s="1">
+        <v>2007</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>68</v>
+        <v>292</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.74</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="J3" s="1">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>65</v>
+        <v>294</v>
       </c>
       <c r="L3" s="1">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="2">
-        <v>143533</v>
-      </c>
-      <c r="O3" s="1">
-        <v>30</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="Q3" s="1">
         <v>80</v>
@@ -1883,80 +1870,80 @@
       <c r="R3" s="1">
         <v>75</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" s="1">
+      <c r="S3" s="1">
+        <v>75</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>80</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>80</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>80</v>
+      </c>
+      <c r="AM3" s="1">
         <v>90</v>
       </c>
-      <c r="U3" s="1">
-        <v>85</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="1">
-        <v>70</v>
-      </c>
-      <c r="X3" s="1">
-        <v>75</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>50</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>40</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>55</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>95</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>35</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI3" s="1">
-        <v>60</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AK3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>26</v>
+      <c r="AN3" s="1">
+        <v>80</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AP3" s="1">
-        <v>70</v>
-      </c>
-      <c r="AQ3" s="1">
-        <v>95</v>
+      <c r="AP3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AR3" s="1">
         <v>80</v>
@@ -1967,65 +1954,193 @@
       <c r="AT3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AU3" s="1">
+      <c r="AU3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AV3" s="1">
+        <v>85</v>
+      </c>
+      <c r="AW3" s="1">
+        <v>70</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="BB3" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="BG3" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="BH3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69" ht="372" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2001</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1.84</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="J4" s="1">
+        <v>75</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="L4" s="1">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="1">
+        <v>60</v>
+      </c>
+      <c r="U4" s="1">
         <v>80</v>
       </c>
-      <c r="AV3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AW3" s="1">
+      <c r="V4" s="1">
+        <v>70</v>
+      </c>
+      <c r="W4" s="1">
+        <v>80</v>
+      </c>
+      <c r="X4" s="1">
+        <v>75</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>50</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>80</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>70</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>75</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>60</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>80</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>80</v>
+      </c>
+      <c r="AL4" s="1">
         <v>90</v>
       </c>
-      <c r="AX3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AY3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="BA3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="BB3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BC3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BD3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BE3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BF3" s="1" t="s">
+      <c r="AM4" s="1">
         <v>80</v>
       </c>
-      <c r="BG3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BH3" s="1">
-        <v>2</v>
-      </c>
-      <c r="BI3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BJ3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BL3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BM3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN3" s="1" t="s">
-        <v>52</v>
+      <c r="AN4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AY4" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AZ4" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>305</v>
+      </c>
+      <c r="BH4" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2038,8 +2153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2058,201 +2173,201 @@
   <sheetData>
     <row r="1" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" t="s">
+        <v>107</v>
+      </c>
+      <c r="S1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" t="s">
+        <v>100</v>
+      </c>
+      <c r="U1" t="s">
+        <v>95</v>
+      </c>
+      <c r="V1" t="s">
         <v>96</v>
-      </c>
-      <c r="G1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I1" t="s">
-        <v>120</v>
-      </c>
-      <c r="J1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K1" t="s">
-        <v>135</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="M1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N1" t="s">
-        <v>102</v>
-      </c>
-      <c r="O1" t="s">
-        <v>103</v>
-      </c>
-      <c r="P1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>110</v>
-      </c>
-      <c r="R1" t="s">
-        <v>118</v>
-      </c>
-      <c r="S1" t="s">
-        <v>105</v>
-      </c>
-      <c r="T1" t="s">
-        <v>111</v>
-      </c>
-      <c r="U1" t="s">
-        <v>106</v>
-      </c>
-      <c r="V1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="E2">
         <v>49</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="J2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="K2" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="M2" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="E3">
         <v>45</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="G3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="H3" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="I3" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="M3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>132</v>
       </c>
       <c r="E4">
         <v>49</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="H4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" t="s">
         <v>125</v>
       </c>
-      <c r="I4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J4" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" t="s">
-        <v>136</v>
-      </c>
       <c r="L4" s="6" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="M4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="U4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="V4" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D5" s="9">
         <v>27095</v>
@@ -2261,30 +2376,30 @@
         <v>50</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="G5" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="H5" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="I5" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="J5" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D6" s="9">
         <v>23070</v>
@@ -2293,36 +2408,36 @@
         <v>61</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="H6" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="I6" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="J6" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="K6" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="M6" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D7" s="9">
         <v>29411</v>
@@ -2331,30 +2446,30 @@
         <v>43</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G7" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H7" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="I7" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="M7" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="22.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D8" s="10">
         <v>29575</v>
@@ -2363,33 +2478,33 @@
         <v>43</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="H8" t="s">
-        <v>225</v>
+        <v>287</v>
       </c>
       <c r="I8" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="M8" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D9" s="9">
         <v>23788</v>
@@ -2398,39 +2513,39 @@
         <v>59</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G9" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="H9" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="I9" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="J9" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="K9" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="M9" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D10" s="10">
         <v>24546</v>
@@ -2439,36 +2554,36 @@
         <v>57</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G10" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="H10" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="I10" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="K10" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="M10" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D11" s="10">
         <v>20656</v>
@@ -2477,59 +2592,59 @@
         <v>67</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="G11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H11" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="I11" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="E12">
         <v>47</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G12" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="H12" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="J12" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="K12" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D13" s="10">
         <v>28041</v>
@@ -2538,30 +2653,30 @@
         <v>47</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="G13" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="H13" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="I13" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="J13" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D14" s="10">
         <v>29744</v>
@@ -2570,30 +2685,30 @@
         <v>43</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="G14" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="H14" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="I14" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="J14" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D15" s="10">
         <v>28734</v>
@@ -2602,45 +2717,45 @@
         <v>45</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="G15" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="H15" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="I15" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="J15" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K15" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="M15" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="O15" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D16" s="10">
         <v>29596</v>
@@ -2649,27 +2764,27 @@
         <v>43</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="G16" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="H16" t="s">
-        <v>227</v>
+        <v>288</v>
       </c>
       <c r="I16" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D17" s="10">
         <v>22413</v>
@@ -2678,27 +2793,27 @@
         <v>63</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="G17" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="H17" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="I17" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D18" s="10">
         <v>29431</v>
@@ -2707,30 +2822,30 @@
         <v>43</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G18" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="H18" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="I18" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="K18" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D19" s="10">
         <v>29957</v>
@@ -2739,27 +2854,27 @@
         <v>42</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="G19" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="H19" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="I19" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D20" s="10">
         <v>27245</v>
@@ -2768,30 +2883,30 @@
         <v>49</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="G20" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="H20" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="J20" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="K20" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D21" s="10">
         <v>20554</v>
@@ -2800,30 +2915,30 @@
         <v>68</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="G21" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="H21" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="I21" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="M21" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D22" s="10">
         <v>30562</v>
@@ -2832,24 +2947,24 @@
         <v>40</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G22" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="H22" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D23" s="10">
         <v>21837</v>
@@ -2858,33 +2973,33 @@
         <v>64</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="G23" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="H23" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="I23" t="s">
+        <v>233</v>
+      </c>
+      <c r="J23" t="s">
+        <v>267</v>
+      </c>
+      <c r="M23" t="s">
         <v>246</v>
-      </c>
-      <c r="J23" t="s">
-        <v>280</v>
-      </c>
-      <c r="M23" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D24" s="10">
         <v>29720</v>
@@ -2893,24 +3008,24 @@
         <v>43</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="G24" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="H24" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D25" s="10">
         <v>26682</v>
@@ -2919,24 +3034,24 @@
         <v>51</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G25" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="H25" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D26" s="10">
         <v>29786</v>
@@ -2945,48 +3060,48 @@
         <v>42</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G26" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="H26" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="J26" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="E27">
         <v>43</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="G27" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="H27" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="I27" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="K27" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
agregar jugadores en excel y modificacion de nombres de escudos parte2
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BD8E7A-B0FE-7046-8EFE-58AF412059D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AB2FBC-3A50-B540-90BC-B3E4B95DA56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
@@ -1372,7 +1372,7 @@
   <dimension ref="A1:BQ4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
agregar jugadores en excel y modificacion de nombres de escudos parte3
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AB2FBC-3A50-B540-90BC-B3E4B95DA56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B94294-5B65-F044-B4E7-16CB854D066C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
@@ -1371,7 +1371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
agregar jugadores en excel y modificacion de nombres de escudos parte4
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B94294-5B65-F044-B4E7-16CB854D066C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90154D81-06BD-7F48-9D4F-A47432A5B0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="309">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -979,6 +979,12 @@
   </si>
   <si>
     <t>Controles y perfiles para darle continuidad a la jugada. Vision y precision para colocar pases en ventaja. Engaños corporales y habilidad para recibir y girar rápidamente, conducciones en velocidad. Tranquilidad bajo presión, sale gambeta corta.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LfwfDfrkfnI</t>
+  </si>
+  <si>
+    <t>https://youtu.be/fIelATahlk4</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -2153,8 +2159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2699,6 +2705,9 @@
       <c r="J14" t="s">
         <v>268</v>
       </c>
+      <c r="M14" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="15" spans="1:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -3102,6 +3111,9 @@
       </c>
       <c r="K27" t="s">
         <v>261</v>
+      </c>
+      <c r="M27" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
agregar jugadores en excel y modificacion de nombres de escudos parte5
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90154D81-06BD-7F48-9D4F-A47432A5B0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F29216A-348D-4C48-A804-85D357494145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
@@ -2160,7 +2160,7 @@
   <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Agrego switch de comentario para correr de manera local, excel LOCAL y correccion de Video Compacto en Jugadores
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F29216A-348D-4C48-A804-85D357494145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6A1320-06E5-5C4C-86C6-01DAF3B9BEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="311">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -943,9 +943,6 @@
     <t>17/02/2007</t>
   </si>
   <si>
-    <t>lorenzoalbarracin</t>
-  </si>
-  <si>
     <t>https://youtu.be/x0v6x-e6lu4</t>
   </si>
   <si>
@@ -965,9 +962,6 @@
   </si>
   <si>
     <t>Gonzalo Lagos</t>
-  </si>
-  <si>
-    <t>agustinlagos</t>
   </si>
   <si>
     <t>Intervino en todas las fases de juego, tanto en defensa como en la gestación y en la creación del ataque. Es un lateral con gran claridad en el último tercio, con capacidad de pases interiores. Gran técnica en asociaciones en espacios reducidos y en 1 vs 1. Envia centros de primera y en velocidad lo cual es un recurso que sobresale sobre los demás laterales. Es de talla alta y buen porte, gana duelos aeres y es agerrido en la marca. Entiendo los momentos para saltar a la marca. Le faltaría corregir los momentos cuando pasar al ataque ya que deja muchas veces la marca a las espaldas sin tener un espacio claro donde atacar.
@@ -985,6 +979,18 @@
   </si>
   <si>
     <t>https://youtu.be/fIelATahlk4</t>
+  </si>
+  <si>
+    <t>Argentinos</t>
+  </si>
+  <si>
+    <t>Tallers</t>
+  </si>
+  <si>
+    <t>Diego_Armando_Maradona</t>
+  </si>
+  <si>
+    <t>Facundo_Bernal</t>
   </si>
 </sst>
 </file>
@@ -1377,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1821,96 +1827,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:69" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:69" ht="152" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>291</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>172</v>
+        <v>127</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="1">
-        <v>2007</v>
+        <v>2001</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>292</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="H3" s="1">
-        <v>1.74</v>
+        <v>1.84</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>44</v>
+        <v>298</v>
       </c>
       <c r="J3" s="1">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="L3" s="1">
-        <v>17</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="1">
+        <v>20</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="1">
+        <v>60</v>
+      </c>
+      <c r="U3" s="1">
         <v>80</v>
       </c>
-      <c r="R3" s="1">
+      <c r="V3" s="1">
+        <v>70</v>
+      </c>
+      <c r="W3" s="1">
+        <v>80</v>
+      </c>
+      <c r="X3" s="1">
         <v>75</v>
       </c>
-      <c r="S3" s="1">
+      <c r="Y3" s="1">
+        <v>50</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>80</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>70</v>
+      </c>
+      <c r="AB3" s="1">
         <v>75</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>26</v>
+      <c r="AC3" s="1">
+        <v>60</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>80</v>
       </c>
       <c r="AE3" s="1" t="s">
         <v>26</v>
@@ -1927,20 +1933,20 @@
       <c r="AI3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AJ3" s="1">
-        <v>80</v>
+      <c r="AJ3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AK3" s="1">
         <v>80</v>
       </c>
       <c r="AL3" s="1">
+        <v>90</v>
+      </c>
+      <c r="AM3" s="1">
         <v>80</v>
       </c>
-      <c r="AM3" s="1">
-        <v>90</v>
-      </c>
-      <c r="AN3" s="1">
-        <v>80</v>
+      <c r="AN3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>26</v>
@@ -1951,8 +1957,8 @@
       <c r="AQ3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AR3" s="1">
-        <v>80</v>
+      <c r="AR3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AS3" s="1" t="s">
         <v>26</v>
@@ -1963,149 +1969,149 @@
       <c r="AU3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AV3" s="1">
-        <v>85</v>
-      </c>
-      <c r="AW3" s="1">
-        <v>70</v>
+      <c r="AV3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>212</v>
+        <v>308</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="BB3" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="BG3" s="1" t="s">
-        <v>296</v>
+        <v>302</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>303</v>
       </c>
       <c r="BH3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:69" ht="372" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:69" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>291</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="1">
-        <v>2001</v>
+        <v>2007</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>64</v>
+        <v>292</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H4" s="1">
-        <v>1.84</v>
+        <v>1.74</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>299</v>
+        <v>44</v>
       </c>
       <c r="J4" s="1">
+        <v>72</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="L4" s="1">
+        <v>17</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>80</v>
+      </c>
+      <c r="R4" s="1">
         <v>75</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="L4" s="1">
-        <v>20</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="1">
-        <v>1</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="1">
-        <v>60</v>
-      </c>
-      <c r="U4" s="1">
+      <c r="S4" s="1">
+        <v>75</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ4" s="1">
         <v>80</v>
-      </c>
-      <c r="V4" s="1">
-        <v>70</v>
-      </c>
-      <c r="W4" s="1">
-        <v>80</v>
-      </c>
-      <c r="X4" s="1">
-        <v>75</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>50</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>80</v>
-      </c>
-      <c r="AA4" s="1">
-        <v>70</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>75</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>60</v>
-      </c>
-      <c r="AD4" s="1">
-        <v>80</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="AK4" s="1">
         <v>80</v>
       </c>
       <c r="AL4" s="1">
+        <v>80</v>
+      </c>
+      <c r="AM4" s="1">
         <v>90</v>
       </c>
-      <c r="AM4" s="1">
+      <c r="AN4" s="1">
         <v>80</v>
       </c>
-      <c r="AN4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="AO4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2115,8 +2121,8 @@
       <c r="AQ4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AR4" s="1" t="s">
-        <v>26</v>
+      <c r="AR4" s="1">
+        <v>80</v>
       </c>
       <c r="AS4" s="1" t="s">
         <v>26</v>
@@ -2127,23 +2133,23 @@
       <c r="AU4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AV4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AW4" s="1" t="s">
-        <v>26</v>
+      <c r="AV4" s="1">
+        <v>85</v>
+      </c>
+      <c r="AW4" s="1">
+        <v>70</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>240</v>
+        <v>307</v>
       </c>
       <c r="AY4" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AZ4" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="BB4" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="BG4" t="s">
-        <v>305</v>
+      <c r="BG4" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="BH4" s="1">
         <v>0</v>
@@ -2159,7 +2165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71EAA4-DB9A-434D-BCE1-A1FF79FB8ADD}">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
@@ -2706,7 +2712,7 @@
         <v>268</v>
       </c>
       <c r="M14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -3113,7 +3119,7 @@
         <v>261</v>
       </c>
       <c r="M27" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
modificacion source_informes, agrego Lagos pero estan mal los nombres de los escudos y jugadores
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6A1320-06E5-5C4C-86C6-01DAF3B9BEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5E2928-D0DE-4B4F-957A-A25F73494E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="308">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -981,16 +981,7 @@
     <t>https://youtu.be/fIelATahlk4</t>
   </si>
   <si>
-    <t>Argentinos</t>
-  </si>
-  <si>
-    <t>Tallers</t>
-  </si>
-  <si>
-    <t>Diego_Armando_Maradona</t>
-  </si>
-  <si>
-    <t>Facundo_Bernal</t>
+    <t>0/0/0000</t>
   </si>
 </sst>
 </file>
@@ -1383,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F602D-DF59-584F-8375-3BF517980F50}">
   <dimension ref="A1:BQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AX4" sqref="AX4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1976,10 +1967,10 @@
         <v>26</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>308</v>
+        <v>77</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>310</v>
+        <v>78</v>
       </c>
       <c r="BB3" s="11" t="s">
         <v>302</v>
@@ -2029,13 +2020,13 @@
         <v>17</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>26</v>
+        <v>307</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
+      <c r="O4" s="1">
+        <v>1</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>26</v>
@@ -2140,10 +2131,10 @@
         <v>70</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>307</v>
+        <v>77</v>
       </c>
       <c r="AY4" s="1" t="s">
-        <v>309</v>
+        <v>78</v>
       </c>
       <c r="BB4" s="11" t="s">
         <v>304</v>

</xml_diff>

<commit_message>
branch de pestanias_jugadores desarrolalda
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6A1320-06E5-5C4C-86C6-01DAF3B9BEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F585D95-7F75-5B40-9348-65DA86B22ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="308">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -981,16 +981,7 @@
     <t>https://youtu.be/fIelATahlk4</t>
   </si>
   <si>
-    <t>Argentinos</t>
-  </si>
-  <si>
-    <t>Tallers</t>
-  </si>
-  <si>
-    <t>Diego_Armando_Maradona</t>
-  </si>
-  <si>
-    <t>Facundo_Bernal</t>
+    <t>0/0/0000</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1375,7 @@
   <dimension ref="A1:BQ4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1976,10 +1967,10 @@
         <v>26</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>308</v>
+        <v>77</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>310</v>
+        <v>78</v>
       </c>
       <c r="BB3" s="11" t="s">
         <v>302</v>
@@ -2029,13 +2020,13 @@
         <v>17</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>26</v>
+        <v>307</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
+      <c r="O4" s="1">
+        <v>1</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>26</v>
@@ -2140,10 +2131,10 @@
         <v>70</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>307</v>
+        <v>77</v>
       </c>
       <c r="AY4" s="1" t="s">
-        <v>309</v>
+        <v>78</v>
       </c>
       <c r="BB4" s="11" t="s">
         <v>304</v>

</xml_diff>

<commit_message>
agrego valor de Transfermarket como 0
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC9F865-E6D5-4A49-A8CA-F93FF58C4CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F34E55-D800-3F47-8C13-9910DB0653E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="1" activeTab="2" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="1" activeTab="8" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquero" sheetId="3" r:id="rId1"/>
@@ -1339,7 +1339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1409,6 +1409,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3095,7 +3103,7 @@
   <dimension ref="A1:BZ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3324,7 +3332,9 @@
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
+      <c r="P2" s="10">
+        <v>0</v>
+      </c>
       <c r="Q2" s="10"/>
       <c r="R2" s="1" t="s">
         <v>365</v>
@@ -3432,6 +3442,9 @@
       <c r="M3" t="s">
         <v>341</v>
       </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
       <c r="Q3" t="s">
         <v>390</v>
       </c>
@@ -3472,7 +3485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C0A3C3-E1ED-1A45-B7FE-54727AF59BDE}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -3644,7 +3657,7 @@
   <dimension ref="A1:AX4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3841,6 +3854,9 @@
       <c r="N2" s="20">
         <v>39082</v>
       </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
       <c r="Q2" t="s">
         <v>330</v>
       </c>
@@ -3891,6 +3907,9 @@
       </c>
       <c r="M3" t="s">
         <v>311</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>324</v>
@@ -3930,7 +3949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6334F358-6715-B14E-B754-1BFE6F886067}">
   <dimension ref="A1:AW1"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
@@ -4098,8 +4117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CCB103-BEBB-1C4E-8FD0-99DD5CB959EE}">
   <dimension ref="A1:AX3"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4296,6 +4315,9 @@
       <c r="M2" t="s">
         <v>341</v>
       </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
       <c r="R2" t="s">
         <v>179</v>
       </c>
@@ -4324,8 +4346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2401B5-FAE5-0049-84FC-5A622F2B9171}">
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4513,6 +4535,9 @@
       <c r="M2" t="s">
         <v>383</v>
       </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
       <c r="R2" t="s">
         <v>164</v>
       </c>
@@ -4565,6 +4590,9 @@
       </c>
       <c r="M3" t="s">
         <v>383</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>187</v>
@@ -4593,12 +4621,13 @@
   <dimension ref="A1:AU59"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.2">
@@ -4786,7 +4815,9 @@
         <v>312</v>
       </c>
       <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="P2" s="27">
+        <v>0</v>
+      </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1" t="s">
         <v>296</v>
@@ -4886,7 +4917,9 @@
         <v>312</v>
       </c>
       <c r="O3" s="1"/>
-      <c r="P3" s="2"/>
+      <c r="P3" s="27">
+        <v>0</v>
+      </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
         <v>187</v>
@@ -4951,7 +4984,9 @@
         <v>312</v>
       </c>
       <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="P4" s="27">
+        <v>0</v>
+      </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1" t="s">
         <v>179</v>
@@ -4990,7 +5025,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="P5" s="27"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -5021,7 +5056,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="P6" s="27"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -5052,7 +5087,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="P7" s="27"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -5083,7 +5118,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="P8" s="27"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -5114,7 +5149,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="P9" s="27"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -5145,7 +5180,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="P10" s="27"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -5176,7 +5211,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
+      <c r="P11" s="27"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -5207,7 +5242,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="P12" s="27"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -5238,7 +5273,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+      <c r="P13" s="27"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -5269,7 +5304,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="P14" s="27"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -5300,7 +5335,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="P15" s="27"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -5331,7 +5366,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="P16" s="27"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -5362,7 +5397,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="P17" s="27"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -5393,7 +5428,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="P18" s="27"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -5424,7 +5459,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+      <c r="P19" s="27"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -5455,7 +5490,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="P20" s="27"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -5486,7 +5521,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
+      <c r="P21" s="27"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -5517,7 +5552,7 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="P22" s="27"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -5548,7 +5583,7 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
+      <c r="P23" s="27"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -5579,7 +5614,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
+      <c r="P24" s="27"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -5610,7 +5645,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
+      <c r="P25" s="27"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
@@ -5641,7 +5676,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
+      <c r="P26" s="27"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -5672,7 +5707,7 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
+      <c r="P27" s="27"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -5703,7 +5738,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
+      <c r="P28" s="27"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -5734,7 +5769,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
+      <c r="P29" s="27"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
@@ -5765,7 +5800,7 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
+      <c r="P30" s="27"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
@@ -5796,7 +5831,7 @@
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
+      <c r="P31" s="27"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
@@ -5827,7 +5862,7 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
+      <c r="P32" s="27"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -5858,7 +5893,7 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
+      <c r="P33" s="27"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
@@ -5889,7 +5924,7 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
+      <c r="P34" s="27"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -5920,7 +5955,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
+      <c r="P35" s="27"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -5951,7 +5986,7 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
+      <c r="P36" s="27"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -5982,7 +6017,7 @@
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
+      <c r="P37" s="27"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
@@ -6013,7 +6048,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
+      <c r="P38" s="27"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
@@ -6044,7 +6079,7 @@
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
+      <c r="P39" s="27"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
@@ -6075,7 +6110,7 @@
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
+      <c r="P40" s="27"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
@@ -6106,7 +6141,7 @@
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
+      <c r="P41" s="27"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
@@ -6137,7 +6172,7 @@
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
+      <c r="P42" s="27"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
@@ -6168,7 +6203,7 @@
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
+      <c r="P43" s="27"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
@@ -6199,7 +6234,7 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
+      <c r="P44" s="27"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
@@ -6230,7 +6265,7 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
+      <c r="P45" s="27"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
@@ -6261,7 +6296,7 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
+      <c r="P46" s="27"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
@@ -6292,7 +6327,7 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
+      <c r="P47" s="27"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
@@ -6323,7 +6358,7 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
+      <c r="P48" s="27"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
@@ -6354,7 +6389,7 @@
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
+      <c r="P49" s="27"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
@@ -6385,7 +6420,7 @@
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
+      <c r="P50" s="27"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
@@ -6416,7 +6451,7 @@
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
+      <c r="P51" s="27"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
@@ -6447,7 +6482,7 @@
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
+      <c r="P52" s="27"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
@@ -6478,7 +6513,7 @@
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
+      <c r="P53" s="27"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
@@ -6509,7 +6544,7 @@
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
+      <c r="P54" s="27"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
@@ -6540,7 +6575,7 @@
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
+      <c r="P55" s="27"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
@@ -6571,7 +6606,7 @@
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
+      <c r="P56" s="27"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
@@ -6602,7 +6637,7 @@
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
+      <c r="P57" s="27"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
@@ -6633,7 +6668,7 @@
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
+      <c r="P58" s="27"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
@@ -6664,7 +6699,7 @@
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
+      <c r="P59" s="27"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
@@ -6689,14 +6724,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E69AA53-C7DC-5440-9E5C-3526E0B4E4F2}">
   <dimension ref="A1:AV4"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="BD3" sqref="BD3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.2">
@@ -6882,6 +6918,9 @@
       <c r="M2" t="s">
         <v>341</v>
       </c>
+      <c r="P2" s="30">
+        <v>0</v>
+      </c>
       <c r="R2" t="s">
         <v>343</v>
       </c>
@@ -6936,7 +6975,9 @@
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="P3" s="29">
+        <v>0</v>
+      </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
         <v>324</v>
@@ -6996,6 +7037,9 @@
       <c r="M4" t="s">
         <v>372</v>
       </c>
+      <c r="P4" s="30">
+        <v>0</v>
+      </c>
       <c r="R4" t="s">
         <v>364</v>
       </c>

</xml_diff>

<commit_message>
empiezo debugeo para transfermarket, borro Arquero y unaf ila de mas
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F34E55-D800-3F47-8C13-9910DB0653E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A4D2D4-E038-1842-8E6D-ED6DB1F54B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="1" activeTab="8" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquero" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="388">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -78,12 +78,6 @@
     <t>Velocidad</t>
   </si>
   <si>
-    <t>Peru</t>
-  </si>
-  <si>
-    <t>Johan Rojas</t>
-  </si>
-  <si>
     <t>Nombre_Video_1</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>Boca Juniors</t>
   </si>
   <si>
-    <t>CD La Equidad</t>
-  </si>
-  <si>
     <t>Nombre_Video_3</t>
   </si>
   <si>
@@ -114,21 +105,12 @@
     <t>Sueldo</t>
   </si>
   <si>
-    <t>1/5/25</t>
-  </si>
-  <si>
-    <t>27/7/03</t>
-  </si>
-  <si>
     <t>Pierna Habil</t>
   </si>
   <si>
     <t>Categoria</t>
   </si>
   <si>
-    <t>Primera</t>
-  </si>
-  <si>
     <t>Division</t>
   </si>
   <si>
@@ -142,18 +124,6 @@
   </si>
   <si>
     <t>Titulo_Video_3</t>
-  </si>
-  <si>
-    <t>CD_La_Equidad</t>
-  </si>
-  <si>
-    <t>Johan_Rojas</t>
-  </si>
-  <si>
-    <t>JRojas_Carrera</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=X16KCiIP0yo&amp;t=8s</t>
   </si>
   <si>
     <t>Vencimiento Contrato</t>
@@ -297,9 +267,6 @@
     <t>https://youtu.be/WcrD4yJgwB0</t>
   </si>
   <si>
-    <t>Octavio Rivero</t>
-  </si>
-  <si>
     <t>Lorenzo Albarracin</t>
   </si>
   <si>
@@ -367,12 +334,6 @@
   </si>
   <si>
     <t>Pelota Detenida</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>Arquero</t>
   </si>
   <si>
     <t>Pasa Paralelo</t>
@@ -1339,7 +1300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1413,10 +1374,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1731,10 +1688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0068BB3B-3D3A-6C48-88F3-F8B3E15CADE2}">
-  <dimension ref="A1:BZ6"/>
+  <dimension ref="A1:AS5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AK1" sqref="AK1:AS1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1760,18 +1717,18 @@
     <col min="45" max="45" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>6</v>
@@ -1780,13 +1737,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>4</v>
@@ -1798,13 +1755,13 @@
         <v>2</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>7</v>
@@ -1813,232 +1770,119 @@
         <v>3</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="AE1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AF1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="AJ1" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AK1" s="13" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AL1" s="13" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AM1" s="13" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="AN1" s="13" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AO1" s="13" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="AP1" s="13" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="AQ1" s="13" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="AR1" s="13" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="AS1" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="10">
-        <v>1.84</v>
-      </c>
-      <c r="K2">
-        <v>75</v>
-      </c>
-      <c r="L2" s="10">
-        <v>28</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="10">
-        <v>4</v>
-      </c>
-      <c r="P2" s="10">
-        <v>80</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10">
-        <v>90</v>
-      </c>
-      <c r="AL2" s="10">
-        <v>80</v>
-      </c>
-      <c r="AM2" s="10">
-        <v>50</v>
-      </c>
-      <c r="AN2" s="10">
-        <v>30</v>
-      </c>
-      <c r="AO2" s="10">
-        <v>100</v>
-      </c>
-      <c r="AP2" s="10">
-        <v>25</v>
-      </c>
-      <c r="AQ2" s="10">
-        <v>88</v>
-      </c>
-      <c r="AR2" s="10">
-        <v>55</v>
-      </c>
-      <c r="AS2" s="10">
-        <v>40</v>
-      </c>
-      <c r="AT2" s="10"/>
-      <c r="AU2" s="10"/>
-      <c r="AV2" s="10"/>
-      <c r="AW2" s="10"/>
-      <c r="AX2" s="10"/>
-      <c r="AY2" s="10"/>
-      <c r="BT2" s="10"/>
-      <c r="BU2" s="10"/>
-      <c r="BV2" s="10"/>
-      <c r="BW2" s="10"/>
-      <c r="BX2" s="10"/>
-      <c r="BY2" s="10"/>
-      <c r="BZ2" s="10"/>
-    </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="B3" s="10"/>
-      <c r="L3" s="10"/>
-    </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-    </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="X6" s="1"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="B2" s="10"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
+      <c r="AJ3" s="10"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="X5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2071,207 +1915,207 @@
     <row r="1" spans="2:29" ht="34" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="L1" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>64</v>
-      </c>
-      <c r="R1" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>51</v>
-      </c>
       <c r="AC1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D2" s="7"/>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="L2">
         <v>49</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" t="s">
         <v>43</v>
       </c>
-      <c r="N2" t="s">
-        <v>53</v>
-      </c>
       <c r="O2" s="6" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="Q2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="R2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="2:29" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="7"/>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="L3">
         <v>45</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="N3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="O3" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="P3" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="T3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:29" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="L4">
         <v>49</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="O4" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="P4" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="Q4" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="R4" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="T4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="AB4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="AC4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D5"/>
       <c r="F5"/>
       <c r="H5" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="K5" s="7">
         <v>27095</v>
@@ -2280,19 +2124,19 @@
         <v>50</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="N5" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="O5" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="P5" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="Q5" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="S5" s="5"/>
     </row>
@@ -2300,13 +2144,13 @@
       <c r="D6"/>
       <c r="F6"/>
       <c r="H6" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J6" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="K6" s="7">
         <v>23070</v>
@@ -2315,39 +2159,39 @@
         <v>61</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="N6" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="O6" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="P6" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="Q6" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="R6" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="S6" s="5"/>
       <c r="T6" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D7"/>
       <c r="F7"/>
       <c r="H7" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J7" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="K7" s="7">
         <v>29411</v>
@@ -2356,33 +2200,33 @@
         <v>43</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="N7" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="O7" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="P7" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="S7" s="5"/>
       <c r="T7" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="2:29" ht="22.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8"/>
       <c r="F8"/>
       <c r="H8" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="K8" s="8">
         <v>29575</v>
@@ -2391,35 +2235,35 @@
         <v>43</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="N8" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O8" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="P8" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="T8" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9"/>
       <c r="F9"/>
       <c r="H9" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J9" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="K9" s="7">
         <v>23788</v>
@@ -2428,41 +2272,41 @@
         <v>59</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="N9" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="O9" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="P9" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="Q9" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="R9" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="T9" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="2:29" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10"/>
       <c r="F10"/>
       <c r="H10" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="K10" s="8">
         <v>24546</v>
@@ -2471,38 +2315,38 @@
         <v>57</v>
       </c>
       <c r="M10" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="N10" t="s">
+        <v>182</v>
+      </c>
+      <c r="O10" t="s">
+        <v>183</v>
+      </c>
+      <c r="P10" t="s">
+        <v>184</v>
+      </c>
+      <c r="R10" t="s">
         <v>185</v>
       </c>
-      <c r="N10" t="s">
-        <v>195</v>
-      </c>
-      <c r="O10" t="s">
-        <v>196</v>
-      </c>
-      <c r="P10" t="s">
-        <v>197</v>
-      </c>
-      <c r="R10" t="s">
-        <v>198</v>
-      </c>
       <c r="S10" s="5" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="T10" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D11"/>
       <c r="F11"/>
       <c r="H11" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J11" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="K11" s="8">
         <v>20656</v>
@@ -2511,16 +2355,16 @@
         <v>67</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="N11" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="O11" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="P11" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="S11" s="5"/>
     </row>
@@ -2528,34 +2372,34 @@
       <c r="D12"/>
       <c r="F12"/>
       <c r="H12" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="I12" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="J12" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="L12">
         <v>47</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="N12" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="O12" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="Q12" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="R12" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="S12" s="5"/>
     </row>
@@ -2563,13 +2407,13 @@
       <c r="D13"/>
       <c r="F13"/>
       <c r="H13" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="I13" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J13" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="K13" s="8">
         <v>28041</v>
@@ -2578,19 +2422,19 @@
         <v>47</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="N13" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="O13" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="P13" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="Q13" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="S13" s="5"/>
     </row>
@@ -2598,13 +2442,13 @@
       <c r="D14"/>
       <c r="F14"/>
       <c r="H14" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="I14" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="J14" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="K14" s="8">
         <v>29744</v>
@@ -2613,36 +2457,36 @@
         <v>43</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="N14" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="O14" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="P14" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="Q14" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="S14" s="5"/>
       <c r="T14" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="2:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D15"/>
       <c r="F15"/>
       <c r="H15" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="I15" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J15" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="K15" s="8">
         <v>28734</v>
@@ -2651,47 +2495,47 @@
         <v>45</v>
       </c>
       <c r="M15" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="N15" t="s">
+        <v>219</v>
+      </c>
+      <c r="O15" t="s">
+        <v>220</v>
+      </c>
+      <c r="P15" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>222</v>
+      </c>
+      <c r="R15" t="s">
+        <v>223</v>
+      </c>
+      <c r="S15" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="N15" t="s">
-        <v>232</v>
-      </c>
-      <c r="O15" t="s">
-        <v>233</v>
-      </c>
-      <c r="P15" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>235</v>
-      </c>
-      <c r="R15" t="s">
-        <v>236</v>
-      </c>
-      <c r="S15" s="5" t="s">
-        <v>237</v>
-      </c>
       <c r="T15" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="V15" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D16"/>
       <c r="F16"/>
       <c r="H16" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="I16" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="J16" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="K16" s="8">
         <v>29596</v>
@@ -2700,16 +2544,16 @@
         <v>43</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="N16" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="O16" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="P16" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="S16" s="5"/>
     </row>
@@ -2717,13 +2561,13 @@
       <c r="D17"/>
       <c r="F17"/>
       <c r="H17" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="I17" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J17" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="K17" s="8">
         <v>22413</v>
@@ -2732,16 +2576,16 @@
         <v>63</v>
       </c>
       <c r="M17" s="18" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="N17" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="O17" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="P17" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="S17" s="5"/>
     </row>
@@ -2749,13 +2593,13 @@
       <c r="D18"/>
       <c r="F18"/>
       <c r="H18" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="I18" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J18" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="K18" s="8">
         <v>29431</v>
@@ -2764,19 +2608,19 @@
         <v>43</v>
       </c>
       <c r="M18" s="18" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="N18" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="O18" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="P18" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="R18" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="S18" s="5"/>
     </row>
@@ -2784,13 +2628,13 @@
       <c r="D19"/>
       <c r="F19"/>
       <c r="H19" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="I19" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J19" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="K19" s="8">
         <v>29957</v>
@@ -2799,16 +2643,16 @@
         <v>42</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="N19" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="O19" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="P19" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="S19" s="5"/>
     </row>
@@ -2816,13 +2660,13 @@
       <c r="D20"/>
       <c r="F20"/>
       <c r="H20" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="I20" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J20" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="K20" s="8">
         <v>27245</v>
@@ -2831,19 +2675,19 @@
         <v>49</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="N20" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="O20" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="Q20" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="R20" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="S20" s="5"/>
     </row>
@@ -2851,13 +2695,13 @@
       <c r="D21"/>
       <c r="F21"/>
       <c r="H21" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="I21" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J21" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="K21" s="8">
         <v>20554</v>
@@ -2866,33 +2710,33 @@
         <v>68</v>
       </c>
       <c r="M21" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="N21" t="s">
         <v>261</v>
       </c>
-      <c r="N21" t="s">
-        <v>274</v>
-      </c>
       <c r="O21" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="P21" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="S21" s="5"/>
       <c r="T21" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D22"/>
       <c r="F22"/>
       <c r="H22" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="I22" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J22" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="K22" s="8">
         <v>30562</v>
@@ -2901,13 +2745,13 @@
         <v>40</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="N22" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="O22" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="S22" s="5"/>
     </row>
@@ -2915,13 +2759,13 @@
       <c r="D23"/>
       <c r="F23"/>
       <c r="H23" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="I23" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J23" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="K23" s="8">
         <v>21837</v>
@@ -2930,36 +2774,36 @@
         <v>64</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="N23" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="O23" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="P23" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="Q23" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="S23" s="5"/>
       <c r="T23" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D24"/>
       <c r="F24"/>
       <c r="H24" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="I24" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J24" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="K24" s="8">
         <v>29720</v>
@@ -2968,13 +2812,13 @@
         <v>43</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="N24" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="O24" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="S24" s="5"/>
     </row>
@@ -2982,13 +2826,13 @@
       <c r="D25"/>
       <c r="F25"/>
       <c r="H25" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="I25" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J25" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="K25" s="8">
         <v>26682</v>
@@ -2997,13 +2841,13 @@
         <v>51</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="N25" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="O25" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="S25" s="5"/>
     </row>
@@ -3011,13 +2855,13 @@
       <c r="D26"/>
       <c r="F26"/>
       <c r="H26" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="I26" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J26" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="K26" s="8">
         <v>29786</v>
@@ -3026,16 +2870,16 @@
         <v>42</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="N26" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="O26" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="Q26" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="S26" s="5"/>
     </row>
@@ -3043,38 +2887,38 @@
       <c r="D27"/>
       <c r="F27"/>
       <c r="H27" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="I27" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J27" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="L27">
         <v>43</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="N27" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="O27" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="P27" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="R27" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="S27" s="5"/>
       <c r="T27" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="4:20" x14ac:dyDescent="0.2">
@@ -3152,16 +2996,16 @@
   <sheetData>
     <row r="1" spans="1:78" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>6</v>
@@ -3170,13 +3014,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>4</v>
@@ -3188,13 +3032,13 @@
         <v>2</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>7</v>
@@ -3203,132 +3047,132 @@
         <v>3</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="AE1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AF1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="AJ1" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AK1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="AO1" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AL1" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM1" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="AN1" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="AO1" s="12" t="s">
-        <v>100</v>
-      </c>
       <c r="AP1" s="12" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="AQ1" s="12" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="AR1" s="12" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="AS1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="AT1" s="12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AU1" s="12" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="E2">
         <v>16</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="H2" s="10">
         <v>2008</v>
       </c>
       <c r="I2" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="K2" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="10"/>
@@ -3337,15 +3181,15 @@
       </c>
       <c r="Q2" s="10"/>
       <c r="R2" s="1" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="10"/>
       <c r="V2" s="10" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="W2" s="10"/>
       <c r="X2" s="10"/>
@@ -3407,58 +3251,58 @@
     </row>
     <row r="3" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="E3">
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="H3">
         <v>2009</v>
       </c>
       <c r="I3" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="J3" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="K3" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="L3" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="M3" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="R3" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="S3" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="V3" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="W3" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="AA3" s="23">
         <v>0</v>
@@ -3496,16 +3340,16 @@
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>6</v>
@@ -3514,13 +3358,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>4</v>
@@ -3532,13 +3376,13 @@
         <v>2</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>7</v>
@@ -3547,103 +3391,103 @@
         <v>3</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="AE1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AF1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="AJ1" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AK1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO1" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AL1" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM1" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="AN1" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="AO1" s="12" t="s">
-        <v>100</v>
-      </c>
       <c r="AP1" s="12" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="AQ1" s="12" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="AR1" s="12" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="AS1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="AT1" s="12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AU1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="AV1" s="12" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="AW1" s="12" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AX1" s="12" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3664,16 +3508,16 @@
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>6</v>
@@ -3682,13 +3526,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>4</v>
@@ -3700,13 +3544,13 @@
         <v>2</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>7</v>
@@ -3715,114 +3559,114 @@
         <v>3</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="AE1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AF1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="AJ1" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AK1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO1" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AL1" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM1" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="AN1" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="AO1" s="12" t="s">
-        <v>100</v>
-      </c>
       <c r="AP1" s="12" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="AQ1" s="12" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="AR1" s="12" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="AS1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="AT1" s="12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AU1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="AV1" s="12" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="AW1" s="12" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AX1" s="12" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:50" ht="340" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D2" s="20">
         <v>38727</v>
@@ -3831,25 +3675,25 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="H2">
         <v>2006</v>
       </c>
       <c r="I2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="K2" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="L2">
         <v>70</v>
       </c>
       <c r="M2" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="N2" s="20">
         <v>39082</v>
@@ -3858,19 +3702,19 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="R2" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="S2" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="V2" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -3878,13 +3722,13 @@
     </row>
     <row r="3" spans="1:50" ht="340" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D3" s="19">
         <v>38386</v>
@@ -3893,35 +3737,35 @@
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1">
         <v>2005</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="M3" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="V3" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -3960,16 +3804,16 @@
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>6</v>
@@ -3978,13 +3822,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>4</v>
@@ -3996,13 +3840,13 @@
         <v>2</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>7</v>
@@ -4011,100 +3855,100 @@
         <v>3</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="AE1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AF1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="AJ1" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AK1" s="12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AL1" s="12" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="AM1" s="12" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="AN1" s="12" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="AO1" s="12" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="AP1" s="12" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="AQ1" s="12" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="AR1" s="12" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="AS1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="AT1" s="12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AU1" s="12" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="AV1" s="12" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="AW1" s="12" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -4115,10 +3959,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CCB103-BEBB-1C4E-8FD0-99DD5CB959EE}">
-  <dimension ref="A1:AX3"/>
+  <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4128,16 +3972,16 @@
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>6</v>
@@ -4146,13 +3990,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>4</v>
@@ -4164,13 +4008,13 @@
         <v>2</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>7</v>
@@ -4179,100 +4023,100 @@
         <v>3</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="AE1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AF1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="AJ1" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AK1" s="12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AL1" s="12" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="AM1" s="12" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="AN1" s="12" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="AO1" s="12" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="AP1" s="12" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="AQ1" s="12" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="AR1" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="AS1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="AT1" s="12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AU1" s="12" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="AV1" s="12" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="AW1" s="12" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="AX1" s="12" t="s">
         <v>9</v>
@@ -4280,13 +4124,13 @@
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D2" s="20">
         <v>39917</v>
@@ -4295,44 +4139,39 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="H2">
         <v>2009</v>
       </c>
       <c r="I2" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="J2" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="K2" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="L2">
         <v>50</v>
       </c>
       <c r="M2" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="S2" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="V2" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="AA2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="AA3">
         <v>0</v>
       </c>
     </row>
@@ -4357,16 +4196,16 @@
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>6</v>
@@ -4375,13 +4214,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>4</v>
@@ -4393,13 +4232,13 @@
         <v>2</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>7</v>
@@ -4408,105 +4247,105 @@
         <v>3</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="AE1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AF1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="AJ1" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AK1" s="12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AL1" s="12" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="AM1" s="12" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="AN1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="AO1" s="12" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="AP1" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="AQ1" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="AQ1" s="12" t="s">
-        <v>123</v>
-      </c>
       <c r="AR1" s="12" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="AS1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="AT1" s="12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AU1" s="12" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D2" s="20">
         <v>39487</v>
@@ -4515,40 +4354,40 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="H2">
         <v>2008</v>
       </c>
       <c r="I2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="K2" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="L2">
         <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="S2" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="V2" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="W2" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -4556,13 +4395,13 @@
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D3" s="20">
         <v>38838</v>
@@ -4571,40 +4410,40 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="H3">
         <v>2006</v>
       </c>
       <c r="I3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="K3" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="L3">
         <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="S3" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="V3" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="W3" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -4632,16 +4471,16 @@
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>6</v>
@@ -4650,13 +4489,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>4</v>
@@ -4668,13 +4507,13 @@
         <v>2</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>7</v>
@@ -4683,64 +4522,64 @@
         <v>3</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="AE1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AF1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="AJ1" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AK1" s="12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AL1" s="12" t="s">
         <v>8</v>
@@ -4749,70 +4588,70 @@
         <v>9</v>
       </c>
       <c r="AN1" s="12" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="AO1" s="12" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="AP1" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="AQ1" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="AQ1" s="12" t="s">
-        <v>123</v>
-      </c>
       <c r="AR1" s="12" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="AS1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="AT1" s="12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AU1" s="12" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:47" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1">
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1">
         <v>2007</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="L2" s="1">
         <v>69</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="27">
@@ -4820,18 +4659,18 @@
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -4877,13 +4716,13 @@
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D3" s="19">
         <v>38518</v>
@@ -4892,29 +4731,29 @@
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1">
         <v>2005</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="L3" s="1">
         <v>70</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="27">
@@ -4922,18 +4761,18 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -4946,13 +4785,13 @@
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D4" s="19">
         <v>39580</v>
@@ -4961,27 +4800,27 @@
         <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1">
         <v>2008</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="27">
@@ -4989,15 +4828,15 @@
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -6724,7 +6563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E69AA53-C7DC-5440-9E5C-3526E0B4E4F2}">
   <dimension ref="A1:AV4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="P2" sqref="P2:P1048576"/>
     </sheetView>
   </sheetViews>
@@ -6732,21 +6571,20 @@
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1640625" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>6</v>
@@ -6755,13 +6593,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>4</v>
@@ -6773,13 +6611,13 @@
         <v>2</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>7</v>
@@ -6788,108 +6626,108 @@
         <v>3</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="AE1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AF1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="AJ1" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AK1" s="12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AL1" s="12" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="AM1" s="12" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="AN1" s="12" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="AO1" s="12" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AP1" s="12" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="AQ1" s="12" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="AR1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="AS1" s="12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AT1" s="12" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="AU1" s="12" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="AV1" s="12" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D2" s="20">
         <v>38793</v>
@@ -6898,40 +6736,40 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="H2">
         <v>2006</v>
       </c>
       <c r="I2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="K2" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="L2">
         <v>70</v>
       </c>
       <c r="M2" t="s">
-        <v>341</v>
-      </c>
-      <c r="P2" s="30">
+        <v>328</v>
+      </c>
+      <c r="P2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="S2" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="V2" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="W2" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="AA2" s="24">
         <v>0</v>
@@ -6939,13 +6777,13 @@
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D3" s="19">
         <v>70</v>
@@ -6954,44 +6792,44 @@
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1">
         <v>2005</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="29">
+      <c r="P3" s="1">
         <v>0</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="W3" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -7002,13 +6840,13 @@
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="B4" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D4" s="20">
         <v>38891</v>
@@ -7017,37 +6855,37 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="H4">
         <v>2006</v>
       </c>
       <c r="I4" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="J4" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="K4" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="L4">
         <v>75</v>
       </c>
       <c r="M4" t="s">
-        <v>372</v>
-      </c>
-      <c r="P4" s="30">
+        <v>359</v>
+      </c>
+      <c r="P4">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="S4" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="V4" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="AA4" s="24">
         <v>0</v>

</xml_diff>

<commit_message>
empiezo debugeo para transfermarket, modifico nombres de posiciones para graficar
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A4D2D4-E038-1842-8E6D-ED6DB1F54B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354715C8-765A-F744-AA87-AEF24DE47D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquero" sheetId="3" r:id="rId1"/>
@@ -1690,7 +1690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0068BB3B-3D3A-6C48-88F3-F8B3E15CADE2}">
   <dimension ref="A1:AS5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="AF1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2946,8 +2946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4D60BB-91C5-904F-8458-C1FB9007F945}">
   <dimension ref="A1:BZ4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4185,7 +4185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2401B5-FAE5-0049-84FC-5A622F2B9171}">
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
@@ -4459,7 +4459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274147EF-AE90-004D-9DE5-714D9C80BF71}">
   <dimension ref="A1:AU59"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
empiezo debugeo para transfermarket, modifico excel para sacar datos mal ingresados
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354715C8-765A-F744-AA87-AEF24DE47D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236C2C0F-DEE8-744B-9265-A14BCB2C7F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="8" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquero" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="382">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -960,9 +960,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Zurda</t>
-  </si>
-  <si>
     <t>31/12/2026</t>
   </si>
   <si>
@@ -975,9 +972,6 @@
     <t>Benjamin Bosch</t>
   </si>
   <si>
-    <t>SUB20</t>
-  </si>
-  <si>
     <t>benjaminbosch</t>
   </si>
   <si>
@@ -1071,9 +1065,6 @@
     <t>juarez</t>
   </si>
   <si>
-    <t>SUB15</t>
-  </si>
-  <si>
     <t>https://youtu.be/hxZ9_oCruAo</t>
   </si>
   <si>
@@ -1107,12 +1098,6 @@
     <t>Gales SUB17</t>
   </si>
   <si>
-    <t>1.80cm</t>
-  </si>
-  <si>
-    <t>80kg</t>
-  </si>
-  <si>
     <t>pablolopez</t>
   </si>
   <si>
@@ -1152,9 +1137,6 @@
     <t>Volante Mixto</t>
   </si>
   <si>
-    <t>8VA</t>
-  </si>
-  <si>
     <t>goytia</t>
   </si>
   <si>
@@ -1176,9 +1158,6 @@
     <t>Volante Ofensivo</t>
   </si>
   <si>
-    <t>Derecha</t>
-  </si>
-  <si>
     <t>acevedo</t>
   </si>
   <si>
@@ -1191,12 +1170,6 @@
     <t>23/03/2009</t>
   </si>
   <si>
-    <t>Octava</t>
-  </si>
-  <si>
-    <t>66kg</t>
-  </si>
-  <si>
     <t>Gustavo Goñi</t>
   </si>
   <si>
@@ -1228,6 +1201,15 @@
   </si>
   <si>
     <t>1.82</t>
+  </si>
+  <si>
+    <t>8va</t>
+  </si>
+  <si>
+    <t>1.80</t>
+  </si>
+  <si>
+    <t>Sub15</t>
   </si>
 </sst>
 </file>
@@ -1690,7 +1672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0068BB3B-3D3A-6C48-88F3-F8B3E15CADE2}">
   <dimension ref="A1:AS5"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2946,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4D60BB-91C5-904F-8458-C1FB9007F945}">
   <dimension ref="A1:BZ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3139,40 +3121,40 @@
     </row>
     <row r="2" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>340</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>343</v>
       </c>
       <c r="E2">
         <v>16</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H2" s="10">
         <v>2008</v>
       </c>
       <c r="I2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="K2" t="s">
-        <v>347</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>348</v>
+        <v>380</v>
+      </c>
+      <c r="L2" s="10">
+        <v>80</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>298</v>
+        <v>354</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="10"/>
@@ -3181,15 +3163,15 @@
       </c>
       <c r="Q2" s="10"/>
       <c r="R2" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="10"/>
       <c r="V2" s="10" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="W2" s="10"/>
       <c r="X2" s="10"/>
@@ -3251,7 +3233,7 @@
     </row>
     <row r="3" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s">
         <v>260</v>
@@ -3260,49 +3242,49 @@
         <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="E3">
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H3">
         <v>2009</v>
       </c>
       <c r="I3" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="J3" t="s">
         <v>297</v>
       </c>
       <c r="K3" t="s">
-        <v>347</v>
-      </c>
-      <c r="L3" t="s">
-        <v>376</v>
+        <v>380</v>
+      </c>
+      <c r="L3">
+        <v>66</v>
       </c>
       <c r="M3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="R3" t="s">
         <v>262</v>
       </c>
       <c r="S3" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="V3" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="W3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AA3" s="23">
         <v>0</v>
@@ -3501,7 +3483,7 @@
   <dimension ref="A1:AX4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3660,7 +3642,7 @@
     </row>
     <row r="2" spans="1:50" ht="340" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B2" t="s">
         <v>270</v>
@@ -3675,7 +3657,7 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H2">
         <v>2006</v>
@@ -3684,16 +3666,16 @@
         <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K2" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="L2">
         <v>70</v>
       </c>
       <c r="M2" t="s">
-        <v>298</v>
+        <v>354</v>
       </c>
       <c r="N2" s="20">
         <v>39082</v>
@@ -3702,19 +3684,19 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
+        <v>315</v>
+      </c>
+      <c r="R2" t="s">
+        <v>316</v>
+      </c>
+      <c r="S2" t="s">
+        <v>318</v>
+      </c>
+      <c r="V2" t="s">
         <v>317</v>
       </c>
-      <c r="R2" t="s">
-        <v>318</v>
-      </c>
-      <c r="S2" t="s">
-        <v>320</v>
-      </c>
-      <c r="V2" t="s">
-        <v>319</v>
-      </c>
       <c r="W2" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -3722,10 +3704,10 @@
     </row>
     <row r="3" spans="1:50" ht="340" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C3" t="s">
         <v>72</v>
@@ -3750,22 +3732,22 @@
         <v>297</v>
       </c>
       <c r="M3" t="s">
-        <v>298</v>
+        <v>354</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="V3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -3961,8 +3943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CCB103-BEBB-1C4E-8FD0-99DD5CB959EE}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4124,7 +4106,7 @@
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s">
         <v>164</v>
@@ -4139,25 +4121,25 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H2">
         <v>2009</v>
       </c>
       <c r="I2" t="s">
-        <v>362</v>
+        <v>379</v>
       </c>
       <c r="J2" t="s">
         <v>297</v>
       </c>
       <c r="K2" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="L2">
         <v>50</v>
       </c>
       <c r="M2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -4166,10 +4148,10 @@
         <v>166</v>
       </c>
       <c r="S2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="V2" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -4185,8 +4167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2401B5-FAE5-0049-84FC-5A622F2B9171}">
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4339,7 +4321,7 @@
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B2" t="s">
         <v>148</v>
@@ -4354,7 +4336,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="H2">
         <v>2008</v>
@@ -4366,13 +4348,13 @@
         <v>297</v>
       </c>
       <c r="K2" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="L2">
         <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>370</v>
+        <v>326</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -4381,13 +4363,13 @@
         <v>151</v>
       </c>
       <c r="S2" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="V2" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="W2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -4395,7 +4377,7 @@
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B3" t="s">
         <v>171</v>
@@ -4410,7 +4392,7 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="H3">
         <v>2006</v>
@@ -4422,13 +4404,13 @@
         <v>297</v>
       </c>
       <c r="K3" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="L3">
         <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>370</v>
+        <v>326</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -4437,13 +4419,13 @@
         <v>174</v>
       </c>
       <c r="S3" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="V3" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="W3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -4459,8 +4441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274147EF-AE90-004D-9DE5-714D9C80BF71}">
   <dimension ref="A1:AU59"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4642,16 +4624,16 @@
         <v>297</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="L2" s="1">
         <v>69</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="27">
@@ -4662,7 +4644,7 @@
         <v>283</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -4716,7 +4698,7 @@
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>171</v>
@@ -4741,19 +4723,19 @@
         <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="L3" s="1">
         <v>70</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="27">
@@ -4764,15 +4746,15 @@
         <v>174</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -4785,7 +4767,7 @@
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>164</v>
@@ -4810,17 +4792,17 @@
         <v>73</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>335</v>
+        <v>381</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="27">
@@ -4831,12 +4813,12 @@
         <v>166</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -6563,8 +6545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E69AA53-C7DC-5440-9E5C-3526E0B4E4F2}">
   <dimension ref="A1:AV4"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6721,10 +6703,10 @@
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>72</v>
@@ -6736,7 +6718,7 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H2">
         <v>2006</v>
@@ -6745,31 +6727,31 @@
         <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K2" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="L2">
         <v>70</v>
       </c>
       <c r="M2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="S2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="V2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="W2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AA2" s="24">
         <v>0</v>
@@ -6777,10 +6759,10 @@
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>72</v>
@@ -6792,7 +6774,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1">
@@ -6805,11 +6787,11 @@
         <v>297</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -6818,18 +6800,18 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="W3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -6840,10 +6822,10 @@
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B4" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>72</v>
@@ -6855,37 +6837,37 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H4">
         <v>2006</v>
       </c>
       <c r="I4" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="J4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K4" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="L4">
         <v>75</v>
       </c>
       <c r="M4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="S4" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="V4" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="AA4" s="24">
         <v>0</v>

</xml_diff>

<commit_message>
primera actualizacion poblada con numeros
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236C2C0F-DEE8-744B-9265-A14BCB2C7F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DD609C-0881-404F-B737-2E53787DAA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="8" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="8" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquero" sheetId="3" r:id="rId1"/>
@@ -1676,30 +1676,30 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.296875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.69921875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="47.5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.296875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -1836,11 +1836,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="B2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
@@ -1863,7 +1863,7 @@
       <c r="AL3" s="10"/>
       <c r="AM3" s="10"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="X5" s="1"/>
     </row>
   </sheetData>
@@ -1880,21 +1880,21 @@
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.19921875" customWidth="1"/>
+    <col min="4" max="4" width="13.296875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5" customWidth="1"/>
-    <col min="10" max="11" width="29.1640625" customWidth="1"/>
+    <col min="10" max="11" width="29.19921875" customWidth="1"/>
     <col min="12" max="12" width="9.5" style="5" customWidth="1"/>
     <col min="20" max="20" width="38.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="H1" t="s">
         <v>29</v>
@@ -1963,7 +1963,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D2" s="7"/>
       <c r="H2" t="s">
         <v>30</v>
@@ -2003,7 +2003,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="2:29" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:29" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D3" s="7"/>
       <c r="H3" t="s">
         <v>47</v>
@@ -2039,7 +2039,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="2:29" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:29" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="7"/>
       <c r="H4" t="s">
         <v>56</v>
@@ -2087,7 +2087,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D5"/>
       <c r="F5"/>
       <c r="H5" t="s">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="S5" s="5"/>
     </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D6"/>
       <c r="F6"/>
       <c r="H6" t="s">
@@ -2163,7 +2163,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D7"/>
       <c r="F7"/>
       <c r="H7" t="s">
@@ -2198,7 +2198,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="2:29" ht="22.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:29" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8"/>
       <c r="F8"/>
       <c r="H8" t="s">
@@ -2235,7 +2235,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9"/>
       <c r="F9"/>
       <c r="H9" t="s">
@@ -2278,7 +2278,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="2:29" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:29" ht="20.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10"/>
       <c r="F10"/>
       <c r="H10" t="s">
@@ -2318,7 +2318,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D11"/>
       <c r="F11"/>
       <c r="H11" t="s">
@@ -2350,7 +2350,7 @@
       </c>
       <c r="S11" s="5"/>
     </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D12"/>
       <c r="F12"/>
       <c r="H12" t="s">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D13"/>
       <c r="F13"/>
       <c r="H13" t="s">
@@ -2420,7 +2420,7 @@
       </c>
       <c r="S13" s="5"/>
     </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D14"/>
       <c r="F14"/>
       <c r="H14" t="s">
@@ -2458,7 +2458,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="2:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:29" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D15"/>
       <c r="F15"/>
       <c r="H15" t="s">
@@ -2507,7 +2507,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D16"/>
       <c r="F16"/>
       <c r="H16" t="s">
@@ -2539,7 +2539,7 @@
       </c>
       <c r="S16" s="5"/>
     </row>
-    <row r="17" spans="4:20" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="D17"/>
       <c r="F17"/>
       <c r="H17" t="s">
@@ -2571,7 +2571,7 @@
       </c>
       <c r="S17" s="5"/>
     </row>
-    <row r="18" spans="4:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D18"/>
       <c r="F18"/>
       <c r="H18" t="s">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="S18" s="5"/>
     </row>
-    <row r="19" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D19"/>
       <c r="F19"/>
       <c r="H19" t="s">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="S19" s="5"/>
     </row>
-    <row r="20" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D20"/>
       <c r="F20"/>
       <c r="H20" t="s">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="S20" s="5"/>
     </row>
-    <row r="21" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D21"/>
       <c r="F21"/>
       <c r="H21" t="s">
@@ -2708,7 +2708,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D22"/>
       <c r="F22"/>
       <c r="H22" t="s">
@@ -2737,7 +2737,7 @@
       </c>
       <c r="S22" s="5"/>
     </row>
-    <row r="23" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D23"/>
       <c r="F23"/>
       <c r="H23" t="s">
@@ -2775,7 +2775,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="24" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D24"/>
       <c r="F24"/>
       <c r="H24" t="s">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="S24" s="5"/>
     </row>
-    <row r="25" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D25"/>
       <c r="F25"/>
       <c r="H25" t="s">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="S25" s="5"/>
     </row>
-    <row r="26" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D26"/>
       <c r="F26"/>
       <c r="H26" t="s">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="S26" s="5"/>
     </row>
-    <row r="27" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D27"/>
       <c r="F27"/>
       <c r="H27" t="s">
@@ -2903,19 +2903,19 @@
         <v>296</v>
       </c>
     </row>
-    <row r="28" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D30"/>
     </row>
-    <row r="31" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D31"/>
     </row>
-    <row r="32" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D32"/>
     </row>
   </sheetData>
@@ -2929,54 +2929,54 @@
   <dimension ref="A1:BZ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="AK6" sqref="A6:AK8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.69921875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.19921875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.69921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.296875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.1640625" style="21"/>
-    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.19921875" style="21"/>
+    <col min="28" max="28" width="18.296875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="13.5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.296875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.796875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:78" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>337</v>
       </c>
@@ -3231,7 +3231,7 @@
       <c r="BY2" s="10"/>
       <c r="BZ2" s="10"/>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>359</v>
       </c>
@@ -3289,8 +3289,41 @@
       <c r="AA3" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.2">
+      <c r="AK3">
+        <v>85</v>
+      </c>
+      <c r="AL3">
+        <v>90</v>
+      </c>
+      <c r="AM3">
+        <v>75</v>
+      </c>
+      <c r="AN3">
+        <v>60</v>
+      </c>
+      <c r="AO3">
+        <v>80</v>
+      </c>
+      <c r="AP3">
+        <v>80</v>
+      </c>
+      <c r="AQ3">
+        <v>80</v>
+      </c>
+      <c r="AR3">
+        <v>95</v>
+      </c>
+      <c r="AS3">
+        <v>85</v>
+      </c>
+      <c r="AT3">
+        <v>80</v>
+      </c>
+      <c r="AU3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
@@ -3315,12 +3348,12 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -3482,13 +3515,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE514E3-04E4-8B46-96A7-6CD9819B7F49}">
   <dimension ref="A1:AX4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="W1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2:AY3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -3640,7 +3673,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:50" ht="340" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" ht="312" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>312</v>
       </c>
@@ -3701,8 +3734,50 @@
       <c r="AA2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:50" ht="340" x14ac:dyDescent="0.2">
+      <c r="AK2">
+        <v>85</v>
+      </c>
+      <c r="AL2">
+        <v>90</v>
+      </c>
+      <c r="AM2">
+        <v>75</v>
+      </c>
+      <c r="AN2">
+        <v>80</v>
+      </c>
+      <c r="AO2">
+        <v>80</v>
+      </c>
+      <c r="AP2">
+        <v>90</v>
+      </c>
+      <c r="AQ2">
+        <v>85</v>
+      </c>
+      <c r="AR2">
+        <v>95</v>
+      </c>
+      <c r="AS2">
+        <v>85</v>
+      </c>
+      <c r="AT2">
+        <v>80</v>
+      </c>
+      <c r="AU2">
+        <v>90</v>
+      </c>
+      <c r="AV2">
+        <v>80</v>
+      </c>
+      <c r="AW2">
+        <v>70</v>
+      </c>
+      <c r="AX2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" ht="312" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>307</v>
       </c>
@@ -3752,8 +3827,50 @@
       <c r="AA3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="AK3">
+        <v>80</v>
+      </c>
+      <c r="AL3">
+        <v>80</v>
+      </c>
+      <c r="AM3">
+        <v>90</v>
+      </c>
+      <c r="AN3">
+        <v>85</v>
+      </c>
+      <c r="AO3">
+        <v>75</v>
+      </c>
+      <c r="AP3">
+        <v>90</v>
+      </c>
+      <c r="AQ3">
+        <v>70</v>
+      </c>
+      <c r="AR3">
+        <v>80</v>
+      </c>
+      <c r="AS3">
+        <v>70</v>
+      </c>
+      <c r="AT3">
+        <v>80</v>
+      </c>
+      <c r="AU3">
+        <v>85</v>
+      </c>
+      <c r="AV3">
+        <v>80</v>
+      </c>
+      <c r="AW3">
+        <v>75</v>
+      </c>
+      <c r="AX3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3779,12 +3896,12 @@
       <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -3943,16 +4060,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CCB103-BEBB-1C4E-8FD0-99DD5CB959EE}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AI30" sqref="AI30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -4104,7 +4221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>355</v>
       </c>
@@ -4155,6 +4272,48 @@
       </c>
       <c r="AA2">
         <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>85</v>
+      </c>
+      <c r="AL2">
+        <v>90</v>
+      </c>
+      <c r="AM2">
+        <v>75</v>
+      </c>
+      <c r="AN2">
+        <v>60</v>
+      </c>
+      <c r="AO2">
+        <v>80</v>
+      </c>
+      <c r="AP2">
+        <v>80</v>
+      </c>
+      <c r="AQ2">
+        <v>80</v>
+      </c>
+      <c r="AR2">
+        <v>95</v>
+      </c>
+      <c r="AS2">
+        <v>85</v>
+      </c>
+      <c r="AT2">
+        <v>80</v>
+      </c>
+      <c r="AU2">
+        <v>90</v>
+      </c>
+      <c r="AV2">
+        <v>70</v>
+      </c>
+      <c r="AW2">
+        <v>85</v>
+      </c>
+      <c r="AX2">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -4167,16 +4326,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2401B5-FAE5-0049-84FC-5A622F2B9171}">
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2:AU3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -4319,7 +4478,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>304</v>
       </c>
@@ -4374,8 +4533,41 @@
       <c r="AA2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AK2">
+        <v>85</v>
+      </c>
+      <c r="AL2">
+        <v>90</v>
+      </c>
+      <c r="AM2">
+        <v>75</v>
+      </c>
+      <c r="AN2">
+        <v>80</v>
+      </c>
+      <c r="AO2">
+        <v>80</v>
+      </c>
+      <c r="AP2">
+        <v>90</v>
+      </c>
+      <c r="AQ2">
+        <v>85</v>
+      </c>
+      <c r="AR2">
+        <v>95</v>
+      </c>
+      <c r="AS2">
+        <v>85</v>
+      </c>
+      <c r="AT2">
+        <v>80</v>
+      </c>
+      <c r="AU2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>305</v>
       </c>
@@ -4429,6 +4621,39 @@
       </c>
       <c r="AA3">
         <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>80</v>
+      </c>
+      <c r="AL3">
+        <v>80</v>
+      </c>
+      <c r="AM3">
+        <v>90</v>
+      </c>
+      <c r="AN3">
+        <v>85</v>
+      </c>
+      <c r="AO3">
+        <v>75</v>
+      </c>
+      <c r="AP3">
+        <v>90</v>
+      </c>
+      <c r="AQ3">
+        <v>70</v>
+      </c>
+      <c r="AR3">
+        <v>80</v>
+      </c>
+      <c r="AS3">
+        <v>70</v>
+      </c>
+      <c r="AT3">
+        <v>80</v>
+      </c>
+      <c r="AU3">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4441,17 +4666,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274147EF-AE90-004D-9DE5-714D9C80BF71}">
   <dimension ref="A1:AU59"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2:AU4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1640625" style="28"/>
+    <col min="16" max="16" width="11.19921875" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -4594,7 +4819,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:47" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>71</v>
       </c>
@@ -4666,19 +4891,19 @@
         <v>90</v>
       </c>
       <c r="AL2">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="AM2">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="AN2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AO2">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="AP2">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="AQ2">
         <v>55</v>
@@ -4687,16 +4912,16 @@
         <v>89</v>
       </c>
       <c r="AS2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="AT2">
         <v>75</v>
       </c>
       <c r="AU2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>301</v>
       </c>
@@ -4764,8 +4989,41 @@
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AK3">
+        <v>85</v>
+      </c>
+      <c r="AL3">
+        <v>90</v>
+      </c>
+      <c r="AM3">
+        <v>75</v>
+      </c>
+      <c r="AN3">
+        <v>60</v>
+      </c>
+      <c r="AO3">
+        <v>80</v>
+      </c>
+      <c r="AP3">
+        <v>80</v>
+      </c>
+      <c r="AQ3">
+        <v>85</v>
+      </c>
+      <c r="AR3">
+        <v>95</v>
+      </c>
+      <c r="AS3">
+        <v>85</v>
+      </c>
+      <c r="AT3">
+        <v>80</v>
+      </c>
+      <c r="AU3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>306</v>
       </c>
@@ -4829,8 +5087,41 @@
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AK4">
+        <v>100</v>
+      </c>
+      <c r="AL4">
+        <v>75</v>
+      </c>
+      <c r="AM4">
+        <v>90</v>
+      </c>
+      <c r="AN4">
+        <v>70</v>
+      </c>
+      <c r="AO4">
+        <v>75</v>
+      </c>
+      <c r="AP4">
+        <v>75</v>
+      </c>
+      <c r="AQ4">
+        <v>45</v>
+      </c>
+      <c r="AR4">
+        <v>95</v>
+      </c>
+      <c r="AS4">
+        <v>80</v>
+      </c>
+      <c r="AT4">
+        <v>80</v>
+      </c>
+      <c r="AU4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4861,7 +5152,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4892,7 +5183,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4923,7 +5214,7 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4954,7 +5245,7 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4985,7 +5276,7 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -5016,7 +5307,7 @@
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -5047,7 +5338,7 @@
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -5078,7 +5369,7 @@
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -5109,7 +5400,7 @@
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -5140,7 +5431,7 @@
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -5171,7 +5462,7 @@
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -5202,7 +5493,7 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -5233,7 +5524,7 @@
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -5264,7 +5555,7 @@
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -5295,7 +5586,7 @@
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -5326,7 +5617,7 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -5357,7 +5648,7 @@
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -5388,7 +5679,7 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -5419,7 +5710,7 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -5450,7 +5741,7 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -5481,7 +5772,7 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -5512,7 +5803,7 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -5543,7 +5834,7 @@
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -5574,7 +5865,7 @@
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -5605,7 +5896,7 @@
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -5636,7 +5927,7 @@
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -5667,7 +5958,7 @@
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -5698,7 +5989,7 @@
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -5729,7 +6020,7 @@
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -5760,7 +6051,7 @@
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -5791,7 +6082,7 @@
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -5822,7 +6113,7 @@
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -5853,7 +6144,7 @@
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -5884,7 +6175,7 @@
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -5915,7 +6206,7 @@
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -5946,7 +6237,7 @@
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -5977,7 +6268,7 @@
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -6008,7 +6299,7 @@
       <c r="AB42" s="1"/>
       <c r="AC42" s="1"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -6039,7 +6330,7 @@
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -6070,7 +6361,7 @@
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -6101,7 +6392,7 @@
       <c r="AB45" s="1"/>
       <c r="AC45" s="1"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -6132,7 +6423,7 @@
       <c r="AB46" s="1"/>
       <c r="AC46" s="1"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -6163,7 +6454,7 @@
       <c r="AB47" s="1"/>
       <c r="AC47" s="1"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -6194,7 +6485,7 @@
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -6225,7 +6516,7 @@
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -6256,7 +6547,7 @@
       <c r="AB50" s="1"/>
       <c r="AC50" s="1"/>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -6287,7 +6578,7 @@
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -6318,7 +6609,7 @@
       <c r="AB52" s="1"/>
       <c r="AC52" s="1"/>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -6349,7 +6640,7 @@
       <c r="AB53" s="1"/>
       <c r="AC53" s="1"/>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -6380,7 +6671,7 @@
       <c r="AB54" s="1"/>
       <c r="AC54" s="1"/>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -6411,7 +6702,7 @@
       <c r="AB55" s="1"/>
       <c r="AC55" s="1"/>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -6442,7 +6733,7 @@
       <c r="AB56" s="1"/>
       <c r="AC56" s="1"/>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -6473,7 +6764,7 @@
       <c r="AB57" s="1"/>
       <c r="AC57" s="1"/>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -6504,7 +6795,7 @@
       <c r="AB58" s="1"/>
       <c r="AC58" s="1"/>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -6545,17 +6836,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E69AA53-C7DC-5440-9E5C-3526E0B4E4F2}">
   <dimension ref="A1:AV4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AV3" sqref="AV3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -6701,7 +6992,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>323</v>
       </c>
@@ -6756,8 +7047,44 @@
       <c r="AA2" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AK2">
+        <v>90</v>
+      </c>
+      <c r="AL2">
+        <v>65</v>
+      </c>
+      <c r="AM2">
+        <v>80</v>
+      </c>
+      <c r="AN2">
+        <v>60</v>
+      </c>
+      <c r="AO2">
+        <v>80</v>
+      </c>
+      <c r="AP2">
+        <v>70</v>
+      </c>
+      <c r="AQ2">
+        <v>70</v>
+      </c>
+      <c r="AR2">
+        <v>89</v>
+      </c>
+      <c r="AS2">
+        <v>70</v>
+      </c>
+      <c r="AT2">
+        <v>75</v>
+      </c>
+      <c r="AU2">
+        <v>85</v>
+      </c>
+      <c r="AV2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>329</v>
       </c>
@@ -6819,8 +7146,44 @@
       <c r="AA3" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AK3">
+        <v>85</v>
+      </c>
+      <c r="AL3">
+        <v>90</v>
+      </c>
+      <c r="AM3">
+        <v>75</v>
+      </c>
+      <c r="AN3">
+        <v>60</v>
+      </c>
+      <c r="AO3">
+        <v>80</v>
+      </c>
+      <c r="AP3">
+        <v>80</v>
+      </c>
+      <c r="AQ3">
+        <v>80</v>
+      </c>
+      <c r="AR3">
+        <v>95</v>
+      </c>
+      <c r="AS3">
+        <v>85</v>
+      </c>
+      <c r="AT3">
+        <v>80</v>
+      </c>
+      <c r="AU3">
+        <v>90</v>
+      </c>
+      <c r="AV3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>350</v>
       </c>
@@ -6871,6 +7234,42 @@
       </c>
       <c r="AA4" s="24">
         <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>90</v>
+      </c>
+      <c r="AL4">
+        <v>75</v>
+      </c>
+      <c r="AM4">
+        <v>90</v>
+      </c>
+      <c r="AN4">
+        <v>70</v>
+      </c>
+      <c r="AO4">
+        <v>90</v>
+      </c>
+      <c r="AP4">
+        <v>75</v>
+      </c>
+      <c r="AQ4">
+        <v>90</v>
+      </c>
+      <c r="AR4">
+        <v>95</v>
+      </c>
+      <c r="AS4">
+        <v>80</v>
+      </c>
+      <c r="AT4">
+        <v>80</v>
+      </c>
+      <c r="AU4">
+        <v>85</v>
+      </c>
+      <c r="AV4">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambio de regate por regates en excel en pestania mixto
</commit_message>
<xml_diff>
--- a/data/source_informes.xlsx
+++ b/data/source_informes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciopastorebenaim/Documents/Python/informes-KBZA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DD609C-0881-404F-B737-2E53787DAA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85D33B9-4428-174F-9F0D-B67F273B25DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="8" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" activeTab="5" xr2:uid="{7F3E787D-03D8-4E4C-8EC3-6093DD8D59D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquero" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="381">
   <si>
     <t>Nacionalidad</t>
   </si>
@@ -376,9 +376,6 @@
   </si>
   <si>
     <t>Duelos defensivos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regate </t>
   </si>
   <si>
     <t>Regates</t>
@@ -1676,30 +1673,30 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.19921875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.69921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="47.5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.69921875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -1719,7 +1716,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>21</v>
@@ -1755,22 +1752,22 @@
         <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>23</v>
@@ -1779,7 +1776,7 @@
         <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>24</v>
@@ -1833,14 +1830,14 @@
         <v>84</v>
       </c>
       <c r="AS1" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
@@ -1863,7 +1860,7 @@
       <c r="AL3" s="10"/>
       <c r="AM3" s="10"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="X5" s="1"/>
     </row>
   </sheetData>
@@ -1880,21 +1877,21 @@
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.19921875" customWidth="1"/>
-    <col min="4" max="4" width="13.296875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="19.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5" customWidth="1"/>
-    <col min="10" max="11" width="29.19921875" customWidth="1"/>
+    <col min="10" max="11" width="29.1640625" customWidth="1"/>
     <col min="12" max="12" width="9.5" style="5" customWidth="1"/>
     <col min="20" max="20" width="38.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:29" ht="34" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
       <c r="H1" t="s">
         <v>29</v>
@@ -1963,7 +1960,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D2" s="7"/>
       <c r="H2" t="s">
         <v>30</v>
@@ -1987,23 +1984,23 @@
         <v>43</v>
       </c>
       <c r="O2" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" t="s">
         <v>132</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>133</v>
-      </c>
-      <c r="R2" t="s">
-        <v>134</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="2:29" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:29" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="7"/>
       <c r="H3" t="s">
         <v>47</v>
@@ -2027,10 +2024,10 @@
         <v>49</v>
       </c>
       <c r="O3" t="s">
+        <v>134</v>
+      </c>
+      <c r="P3" t="s">
         <v>135</v>
-      </c>
-      <c r="P3" t="s">
-        <v>136</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>69</v>
@@ -2039,7 +2036,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="2:29" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:29" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="H4" t="s">
         <v>56</v>
@@ -2063,16 +2060,16 @@
         <v>59</v>
       </c>
       <c r="O4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P4" t="s">
         <v>64</v>
       </c>
       <c r="Q4" t="s">
+        <v>137</v>
+      </c>
+      <c r="R4" t="s">
         <v>138</v>
-      </c>
-      <c r="R4" t="s">
-        <v>139</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>60</v>
@@ -2087,17 +2084,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D5"/>
       <c r="F5"/>
       <c r="H5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I5" t="s">
         <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K5" s="7">
         <v>27095</v>
@@ -2106,33 +2103,33 @@
         <v>50</v>
       </c>
       <c r="M5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="N5" t="s">
         <v>142</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>143</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>144</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>145</v>
       </c>
-      <c r="Q5" t="s">
-        <v>146</v>
-      </c>
       <c r="S5" s="5"/>
     </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D6"/>
       <c r="F6"/>
       <c r="H6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I6" t="s">
         <v>32</v>
       </c>
       <c r="J6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K6" s="7">
         <v>23070</v>
@@ -2141,39 +2138,39 @@
         <v>61</v>
       </c>
       <c r="M6" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="N6" t="s">
         <v>149</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>150</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>151</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>152</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>153</v>
-      </c>
-      <c r="R6" t="s">
-        <v>154</v>
       </c>
       <c r="S6" s="5"/>
       <c r="T6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D7"/>
       <c r="F7"/>
       <c r="H7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I7" t="s">
         <v>32</v>
       </c>
       <c r="J7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K7" s="7">
         <v>29411</v>
@@ -2182,33 +2179,33 @@
         <v>43</v>
       </c>
       <c r="M7" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="N7" t="s">
         <v>158</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>159</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>160</v>
-      </c>
-      <c r="P7" t="s">
-        <v>161</v>
       </c>
       <c r="S7" s="5"/>
       <c r="T7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="2:29" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="2:29" ht="22.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8"/>
       <c r="F8"/>
       <c r="H8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I8" t="s">
         <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K8" s="8">
         <v>29575</v>
@@ -2220,32 +2217,32 @@
         <v>33</v>
       </c>
       <c r="N8" t="s">
+        <v>164</v>
+      </c>
+      <c r="O8" t="s">
         <v>165</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>166</v>
       </c>
-      <c r="P8" t="s">
+      <c r="S8" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="T8" t="s">
         <v>168</v>
       </c>
-      <c r="T8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9"/>
       <c r="F9"/>
       <c r="H9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I9" t="s">
         <v>32</v>
       </c>
       <c r="J9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K9" s="7">
         <v>23788</v>
@@ -2254,41 +2251,41 @@
         <v>59</v>
       </c>
       <c r="M9" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="N9" t="s">
         <v>172</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>173</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>174</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>175</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>176</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="S9" s="5" t="s">
+      <c r="T9" t="s">
         <v>178</v>
       </c>
-      <c r="T9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="2:29" ht="20.55" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:29" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10"/>
       <c r="F10"/>
       <c r="H10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I10" t="s">
         <v>32</v>
       </c>
       <c r="J10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K10" s="8">
         <v>24546</v>
@@ -2297,38 +2294,38 @@
         <v>57</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N10" t="s">
+        <v>181</v>
+      </c>
+      <c r="O10" t="s">
         <v>182</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>183</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>184</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="S10" s="5" t="s">
+      <c r="T10" t="s">
         <v>186</v>
       </c>
-      <c r="T10" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D11"/>
       <c r="F11"/>
       <c r="H11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I11" t="s">
         <v>32</v>
       </c>
       <c r="J11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K11" s="8">
         <v>20656</v>
@@ -2337,65 +2334,65 @@
         <v>67</v>
       </c>
       <c r="M11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N11" t="s">
         <v>190</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>191</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>192</v>
       </c>
-      <c r="P11" t="s">
-        <v>193</v>
-      </c>
       <c r="S11" s="5"/>
     </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D12"/>
       <c r="F12"/>
       <c r="H12" t="s">
+        <v>193</v>
+      </c>
+      <c r="I12" t="s">
         <v>194</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>195</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>197</v>
       </c>
       <c r="L12">
         <v>47</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N12" t="s">
+        <v>197</v>
+      </c>
+      <c r="O12" t="s">
         <v>198</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>199</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>200</v>
       </c>
-      <c r="R12" t="s">
-        <v>201</v>
-      </c>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D13"/>
       <c r="F13"/>
       <c r="H13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I13" t="s">
         <v>32</v>
       </c>
       <c r="J13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K13" s="8">
         <v>28041</v>
@@ -2404,33 +2401,33 @@
         <v>47</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N13" t="s">
+        <v>203</v>
+      </c>
+      <c r="O13" t="s">
         <v>204</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>205</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>206</v>
       </c>
-      <c r="Q13" t="s">
-        <v>207</v>
-      </c>
       <c r="S13" s="5"/>
     </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D14"/>
       <c r="F14"/>
       <c r="H14" t="s">
+        <v>207</v>
+      </c>
+      <c r="I14" t="s">
         <v>208</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>209</v>
-      </c>
-      <c r="J14" t="s">
-        <v>210</v>
       </c>
       <c r="K14" s="8">
         <v>29744</v>
@@ -2439,36 +2436,36 @@
         <v>43</v>
       </c>
       <c r="M14" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="N14" t="s">
         <v>211</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>212</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>213</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>214</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>215</v>
       </c>
       <c r="S14" s="5"/>
       <c r="T14" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="15" spans="2:29" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="2:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D15"/>
       <c r="F15"/>
       <c r="H15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I15" t="s">
         <v>32</v>
       </c>
       <c r="J15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K15" s="8">
         <v>28734</v>
@@ -2477,47 +2474,47 @@
         <v>45</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N15" t="s">
+        <v>218</v>
+      </c>
+      <c r="O15" t="s">
         <v>219</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>220</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>221</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>222</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="S15" s="5" t="s">
+      <c r="T15" t="s">
         <v>224</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="U15" s="5" t="s">
+      <c r="V15" t="s">
         <v>226</v>
       </c>
-      <c r="V15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" spans="2:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="D16"/>
       <c r="F16"/>
       <c r="H16" t="s">
+        <v>227</v>
+      </c>
+      <c r="I16" t="s">
         <v>228</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>229</v>
-      </c>
-      <c r="J16" t="s">
-        <v>230</v>
       </c>
       <c r="K16" s="8">
         <v>29596</v>
@@ -2526,30 +2523,30 @@
         <v>43</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N16" t="s">
+        <v>230</v>
+      </c>
+      <c r="O16" t="s">
         <v>231</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>232</v>
       </c>
-      <c r="P16" t="s">
-        <v>233</v>
-      </c>
       <c r="S16" s="5"/>
     </row>
-    <row r="17" spans="4:20" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:20" ht="34" x14ac:dyDescent="0.2">
       <c r="D17"/>
       <c r="F17"/>
       <c r="H17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I17" t="s">
         <v>32</v>
       </c>
       <c r="J17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K17" s="8">
         <v>22413</v>
@@ -2558,30 +2555,30 @@
         <v>63</v>
       </c>
       <c r="M17" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="N17" t="s">
         <v>236</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>237</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>238</v>
       </c>
-      <c r="P17" t="s">
-        <v>239</v>
-      </c>
       <c r="S17" s="5"/>
     </row>
-    <row r="18" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:20" ht="17" x14ac:dyDescent="0.2">
       <c r="D18"/>
       <c r="F18"/>
       <c r="H18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I18" t="s">
         <v>32</v>
       </c>
       <c r="J18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K18" s="8">
         <v>29431</v>
@@ -2590,33 +2587,33 @@
         <v>43</v>
       </c>
       <c r="M18" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N18" t="s">
+        <v>241</v>
+      </c>
+      <c r="O18" t="s">
         <v>242</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>243</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>244</v>
       </c>
-      <c r="R18" t="s">
-        <v>245</v>
-      </c>
       <c r="S18" s="5"/>
     </row>
-    <row r="19" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D19"/>
       <c r="F19"/>
       <c r="H19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I19" t="s">
         <v>32</v>
       </c>
       <c r="J19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K19" s="8">
         <v>29957</v>
@@ -2625,30 +2622,30 @@
         <v>42</v>
       </c>
       <c r="M19" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="N19" t="s">
         <v>248</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>249</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>250</v>
       </c>
-      <c r="P19" t="s">
-        <v>251</v>
-      </c>
       <c r="S19" s="5"/>
     </row>
-    <row r="20" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D20"/>
       <c r="F20"/>
       <c r="H20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I20" t="s">
         <v>32</v>
       </c>
       <c r="J20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K20" s="8">
         <v>27245</v>
@@ -2657,33 +2654,33 @@
         <v>49</v>
       </c>
       <c r="M20" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="N20" t="s">
         <v>254</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>255</v>
       </c>
-      <c r="O20" t="s">
+      <c r="Q20" t="s">
         <v>256</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>257</v>
       </c>
-      <c r="R20" t="s">
-        <v>258</v>
-      </c>
       <c r="S20" s="5"/>
     </row>
-    <row r="21" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D21"/>
       <c r="F21"/>
       <c r="H21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I21" t="s">
         <v>32</v>
       </c>
       <c r="J21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K21" s="8">
         <v>20554</v>
@@ -2692,33 +2689,33 @@
         <v>68</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N21" t="s">
+        <v>260</v>
+      </c>
+      <c r="O21" t="s">
         <v>261</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>262</v>
-      </c>
-      <c r="P21" t="s">
-        <v>263</v>
       </c>
       <c r="S21" s="5"/>
       <c r="T21" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="22" spans="4:20" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D22"/>
       <c r="F22"/>
       <c r="H22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I22" t="s">
         <v>32</v>
       </c>
       <c r="J22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K22" s="8">
         <v>30562</v>
@@ -2730,24 +2727,24 @@
         <v>58</v>
       </c>
       <c r="N22" t="s">
+        <v>266</v>
+      </c>
+      <c r="O22" t="s">
         <v>267</v>
       </c>
-      <c r="O22" t="s">
-        <v>268</v>
-      </c>
       <c r="S22" s="5"/>
     </row>
-    <row r="23" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D23"/>
       <c r="F23"/>
       <c r="H23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I23" t="s">
         <v>32</v>
       </c>
       <c r="J23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K23" s="8">
         <v>21837</v>
@@ -2756,36 +2753,36 @@
         <v>64</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N23" t="s">
+        <v>270</v>
+      </c>
+      <c r="O23" t="s">
         <v>271</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>272</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>273</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>274</v>
       </c>
       <c r="S23" s="5"/>
       <c r="T23" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="24" spans="4:20" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D24"/>
       <c r="F24"/>
       <c r="H24" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I24" t="s">
         <v>32</v>
       </c>
       <c r="J24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K24" s="8">
         <v>29720</v>
@@ -2794,27 +2791,27 @@
         <v>43</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N24" t="s">
+        <v>277</v>
+      </c>
+      <c r="O24" t="s">
         <v>278</v>
       </c>
-      <c r="O24" t="s">
-        <v>279</v>
-      </c>
       <c r="S24" s="5"/>
     </row>
-    <row r="25" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D25"/>
       <c r="F25"/>
       <c r="H25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I25" t="s">
         <v>32</v>
       </c>
       <c r="J25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K25" s="8">
         <v>26682</v>
@@ -2823,27 +2820,27 @@
         <v>51</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N25" t="s">
+        <v>281</v>
+      </c>
+      <c r="O25" t="s">
         <v>282</v>
       </c>
-      <c r="O25" t="s">
-        <v>283</v>
-      </c>
       <c r="S25" s="5"/>
     </row>
-    <row r="26" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D26"/>
       <c r="F26"/>
       <c r="H26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I26" t="s">
         <v>32</v>
       </c>
       <c r="J26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K26" s="8">
         <v>29786</v>
@@ -2852,70 +2849,70 @@
         <v>42</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N26" t="s">
+        <v>285</v>
+      </c>
+      <c r="O26" t="s">
         <v>286</v>
       </c>
-      <c r="O26" t="s">
+      <c r="Q26" t="s">
         <v>287</v>
       </c>
-      <c r="Q26" t="s">
-        <v>288</v>
-      </c>
       <c r="S26" s="5"/>
     </row>
-    <row r="27" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D27"/>
       <c r="F27"/>
       <c r="H27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I27" t="s">
         <v>32</v>
       </c>
       <c r="J27" t="s">
+        <v>289</v>
+      </c>
+      <c r="K27" s="8" t="s">
         <v>290</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>291</v>
       </c>
       <c r="L27">
         <v>43</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N27" t="s">
+        <v>291</v>
+      </c>
+      <c r="O27" t="s">
         <v>292</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>293</v>
       </c>
-      <c r="P27" t="s">
+      <c r="R27" t="s">
         <v>294</v>
-      </c>
-      <c r="R27" t="s">
-        <v>295</v>
       </c>
       <c r="S27" s="5"/>
       <c r="T27" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="28" spans="4:20" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="28" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D30"/>
     </row>
-    <row r="31" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D31"/>
     </row>
-    <row r="32" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D32"/>
     </row>
   </sheetData>
@@ -2928,55 +2925,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4D60BB-91C5-904F-8458-C1FB9007F945}">
   <dimension ref="A1:BZ4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
       <selection activeCell="AK6" sqref="A6:AK8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="5.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.69921875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.69921875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.19921875" style="21"/>
-    <col min="28" max="28" width="18.296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.1640625" style="21"/>
+    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="13.5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.69921875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.796875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:78" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -2996,7 +2993,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>21</v>
@@ -3032,22 +3029,22 @@
         <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>23</v>
@@ -3056,7 +3053,7 @@
         <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>24</v>
@@ -3095,13 +3092,13 @@
         <v>87</v>
       </c>
       <c r="AN1" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AO1" s="12" t="s">
         <v>89</v>
       </c>
       <c r="AP1" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AQ1" s="12" t="s">
         <v>91</v>
@@ -3119,42 +3116,42 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>339</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>340</v>
       </c>
       <c r="E2">
         <v>16</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H2" s="10">
         <v>2008</v>
       </c>
       <c r="I2" t="s">
+        <v>341</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>343</v>
-      </c>
       <c r="K2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L2" s="10">
         <v>80</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="10"/>
@@ -3163,15 +3160,15 @@
       </c>
       <c r="Q2" s="10"/>
       <c r="R2" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="10"/>
       <c r="V2" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="W2" s="10"/>
       <c r="X2" s="10"/>
@@ -3231,60 +3228,60 @@
       <c r="BY2" s="10"/>
       <c r="BZ2" s="10"/>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C3" t="s">
         <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E3">
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H3">
         <v>2009</v>
       </c>
       <c r="I3" t="s">
+        <v>378</v>
+      </c>
+      <c r="J3" t="s">
+        <v>296</v>
+      </c>
+      <c r="K3" t="s">
         <v>379</v>
-      </c>
-      <c r="J3" t="s">
-        <v>297</v>
-      </c>
-      <c r="K3" t="s">
-        <v>380</v>
       </c>
       <c r="L3">
         <v>66</v>
       </c>
       <c r="M3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3" t="s">
+        <v>367</v>
+      </c>
+      <c r="R3" t="s">
+        <v>261</v>
+      </c>
+      <c r="S3" t="s">
+        <v>365</v>
+      </c>
+      <c r="V3" t="s">
+        <v>359</v>
+      </c>
+      <c r="W3" t="s">
         <v>368</v>
-      </c>
-      <c r="R3" t="s">
-        <v>262</v>
-      </c>
-      <c r="S3" t="s">
-        <v>366</v>
-      </c>
-      <c r="V3" t="s">
-        <v>360</v>
-      </c>
-      <c r="W3" t="s">
-        <v>369</v>
       </c>
       <c r="AA3" s="23">
         <v>0</v>
@@ -3323,7 +3320,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.2">
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
@@ -3344,16 +3341,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C0A3C3-E1ED-1A45-B7FE-54727AF59BDE}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AK1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -3373,7 +3370,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>21</v>
@@ -3409,22 +3406,22 @@
         <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>23</v>
@@ -3433,7 +3430,7 @@
         <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>24</v>
@@ -3515,13 +3512,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE514E3-04E4-8B46-96A7-6CD9819B7F49}">
   <dimension ref="A1:AX4"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="AC1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AK2" sqref="AK2:AY3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -3541,7 +3538,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>21</v>
@@ -3577,22 +3574,22 @@
         <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>23</v>
@@ -3601,7 +3598,7 @@
         <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>24</v>
@@ -3673,12 +3670,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:50" ht="312" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" ht="340" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
@@ -3690,7 +3687,7 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H2">
         <v>2006</v>
@@ -3699,16 +3696,16 @@
         <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L2">
         <v>70</v>
       </c>
       <c r="M2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N2" s="20">
         <v>39082</v>
@@ -3717,19 +3714,19 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
+        <v>314</v>
+      </c>
+      <c r="R2" t="s">
         <v>315</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
+        <v>317</v>
+      </c>
+      <c r="V2" t="s">
         <v>316</v>
       </c>
-      <c r="S2" t="s">
-        <v>318</v>
-      </c>
-      <c r="V2" t="s">
-        <v>317</v>
-      </c>
       <c r="W2" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -3777,12 +3774,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="312" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" ht="340" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" t="s">
         <v>307</v>
-      </c>
-      <c r="B3" t="s">
-        <v>308</v>
       </c>
       <c r="C3" t="s">
         <v>72</v>
@@ -3804,25 +3801,25 @@
         <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="V3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -3870,7 +3867,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3896,12 +3893,12 @@
       <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -3921,7 +3918,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>21</v>
@@ -3957,22 +3954,22 @@
         <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>23</v>
@@ -3981,7 +3978,7 @@
         <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>24</v>
@@ -4060,16 +4057,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CCB103-BEBB-1C4E-8FD0-99DD5CB959EE}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AI30" sqref="AI30"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AW13" sqref="AW13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -4089,7 +4086,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>21</v>
@@ -4125,22 +4122,22 @@
         <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>23</v>
@@ -4149,7 +4146,7 @@
         <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>24</v>
@@ -4191,7 +4188,7 @@
         <v>88</v>
       </c>
       <c r="AO1" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AP1" s="12" t="s">
         <v>107</v>
@@ -4200,7 +4197,7 @@
         <v>103</v>
       </c>
       <c r="AR1" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AS1" s="12" t="s">
         <v>10</v>
@@ -4221,12 +4218,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
@@ -4238,37 +4235,37 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H2">
         <v>2009</v>
       </c>
       <c r="I2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L2">
         <v>50</v>
       </c>
       <c r="M2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="S2" t="s">
+        <v>356</v>
+      </c>
+      <c r="V2" t="s">
         <v>357</v>
-      </c>
-      <c r="V2" t="s">
-        <v>358</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -4326,16 +4323,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2401B5-FAE5-0049-84FC-5A622F2B9171}">
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
+    <sheetView topLeftCell="AI1" workbookViewId="0">
       <selection activeCell="AK2" sqref="AK2:AU3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -4355,7 +4352,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>21</v>
@@ -4391,22 +4388,22 @@
         <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>23</v>
@@ -4415,7 +4412,7 @@
         <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>24</v>
@@ -4457,16 +4454,16 @@
         <v>8</v>
       </c>
       <c r="AO1" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AP1" s="12" t="s">
         <v>97</v>
       </c>
       <c r="AQ1" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AR1" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="AR1" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="AS1" s="12" t="s">
         <v>10</v>
@@ -4475,15 +4472,15 @@
         <v>92</v>
       </c>
       <c r="AU1" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
@@ -4495,7 +4492,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H2">
         <v>2008</v>
@@ -4504,31 +4501,31 @@
         <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L2">
         <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="V2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="W2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -4567,12 +4564,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
         <v>72</v>
@@ -4584,7 +4581,7 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H3">
         <v>2006</v>
@@ -4593,31 +4590,31 @@
         <v>73</v>
       </c>
       <c r="J3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L3">
         <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="V3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="W3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -4670,13 +4667,13 @@
       <selection activeCell="AK2" sqref="AK2:AU4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.19921875" style="28"/>
+    <col min="16" max="16" width="11.1640625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -4696,7 +4693,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>21</v>
@@ -4732,22 +4729,22 @@
         <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>23</v>
@@ -4756,7 +4753,7 @@
         <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>24</v>
@@ -4798,16 +4795,16 @@
         <v>88</v>
       </c>
       <c r="AO1" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AP1" s="12" t="s">
         <v>97</v>
       </c>
       <c r="AQ1" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AR1" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="AR1" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="AS1" s="12" t="s">
         <v>10</v>
@@ -4816,15 +4813,15 @@
         <v>92</v>
       </c>
       <c r="AU1" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>72</v>
@@ -4846,19 +4843,19 @@
         <v>73</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L2" s="1">
         <v>69</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="27">
@@ -4866,10 +4863,10 @@
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -4921,12 +4918,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>72</v>
@@ -4948,19 +4945,19 @@
         <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L3" s="1">
         <v>70</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="27">
@@ -4968,18 +4965,18 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -5023,12 +5020,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>72</v>
@@ -5050,17 +5047,17 @@
         <v>73</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="27">
@@ -5068,15 +5065,15 @@
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -5121,7 +5118,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -5152,7 +5149,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -5183,7 +5180,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -5214,7 +5211,7 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -5245,7 +5242,7 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -5276,7 +5273,7 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -5307,7 +5304,7 @@
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -5338,7 +5335,7 @@
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -5369,7 +5366,7 @@
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -5400,7 +5397,7 @@
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -5431,7 +5428,7 @@
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -5462,7 +5459,7 @@
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -5493,7 +5490,7 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -5524,7 +5521,7 @@
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -5555,7 +5552,7 @@
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -5586,7 +5583,7 @@
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -5617,7 +5614,7 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -5648,7 +5645,7 @@
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -5679,7 +5676,7 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -5710,7 +5707,7 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -5741,7 +5738,7 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -5772,7 +5769,7 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -5803,7 +5800,7 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -5834,7 +5831,7 @@
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -5865,7 +5862,7 @@
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -5896,7 +5893,7 @@
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -5927,7 +5924,7 @@
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -5958,7 +5955,7 @@
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -5989,7 +5986,7 @@
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -6020,7 +6017,7 @@
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -6051,7 +6048,7 @@
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -6082,7 +6079,7 @@
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -6113,7 +6110,7 @@
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -6144,7 +6141,7 @@
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -6175,7 +6172,7 @@
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -6206,7 +6203,7 @@
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -6237,7 +6234,7 @@
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -6268,7 +6265,7 @@
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -6299,7 +6296,7 @@
       <c r="AB42" s="1"/>
       <c r="AC42" s="1"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -6330,7 +6327,7 @@
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -6361,7 +6358,7 @@
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -6392,7 +6389,7 @@
       <c r="AB45" s="1"/>
       <c r="AC45" s="1"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -6423,7 +6420,7 @@
       <c r="AB46" s="1"/>
       <c r="AC46" s="1"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -6454,7 +6451,7 @@
       <c r="AB47" s="1"/>
       <c r="AC47" s="1"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -6485,7 +6482,7 @@
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -6516,7 +6513,7 @@
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -6547,7 +6544,7 @@
       <c r="AB50" s="1"/>
       <c r="AC50" s="1"/>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -6578,7 +6575,7 @@
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -6609,7 +6606,7 @@
       <c r="AB52" s="1"/>
       <c r="AC52" s="1"/>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -6640,7 +6637,7 @@
       <c r="AB53" s="1"/>
       <c r="AC53" s="1"/>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -6671,7 +6668,7 @@
       <c r="AB54" s="1"/>
       <c r="AC54" s="1"/>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -6702,7 +6699,7 @@
       <c r="AB55" s="1"/>
       <c r="AC55" s="1"/>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -6733,7 +6730,7 @@
       <c r="AB56" s="1"/>
       <c r="AC56" s="1"/>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -6764,7 +6761,7 @@
       <c r="AB57" s="1"/>
       <c r="AC57" s="1"/>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -6795,7 +6792,7 @@
       <c r="AB58" s="1"/>
       <c r="AC58" s="1"/>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -6836,17 +6833,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E69AA53-C7DC-5440-9E5C-3526E0B4E4F2}">
   <dimension ref="A1:AV4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+    <sheetView topLeftCell="AN1" workbookViewId="0">
       <selection activeCell="AV3" sqref="AV3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
@@ -6866,7 +6863,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>21</v>
@@ -6902,22 +6899,22 @@
         <v>44</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>23</v>
@@ -6926,7 +6923,7 @@
         <v>53</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>24</v>
@@ -6959,22 +6956,22 @@
         <v>78</v>
       </c>
       <c r="AL1" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AM1" s="12" t="s">
         <v>88</v>
       </c>
       <c r="AN1" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AO1" s="12" t="s">
         <v>97</v>
       </c>
       <c r="AP1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ1" s="12" t="s">
         <v>115</v>
-      </c>
-      <c r="AQ1" s="12" t="s">
-        <v>116</v>
       </c>
       <c r="AR1" s="12" t="s">
         <v>10</v>
@@ -6983,21 +6980,21 @@
         <v>92</v>
       </c>
       <c r="AT1" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AU1" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AV1" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" t="s">
         <v>323</v>
-      </c>
-      <c r="B2" t="s">
-        <v>324</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>72</v>
@@ -7009,7 +7006,7 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H2">
         <v>2006</v>
@@ -7018,31 +7015,31 @@
         <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L2">
         <v>70</v>
       </c>
       <c r="M2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="S2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="W2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AA2" s="24">
         <v>0</v>
@@ -7084,12 +7081,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>72</v>
@@ -7101,7 +7098,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1">
@@ -7111,14 +7108,14 @@
         <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -7127,18 +7124,18 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="W3" t="s">
         <v>330</v>
-      </c>
-      <c r="W3" t="s">
-        <v>331</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -7183,12 +7180,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B4" t="s">
         <v>350</v>
-      </c>
-      <c r="B4" t="s">
-        <v>351</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>72</v>
@@ -7200,37 +7197,37 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H4">
         <v>2006</v>
       </c>
       <c r="I4" t="s">
+        <v>351</v>
+      </c>
+      <c r="J4" t="s">
         <v>352</v>
       </c>
-      <c r="J4" t="s">
-        <v>353</v>
-      </c>
       <c r="K4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L4">
         <v>75</v>
       </c>
       <c r="M4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="V4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AA4" s="24">
         <v>0</v>

</xml_diff>